<commit_message>
skipping filtering out of nonames in pivot
</commit_message>
<xml_diff>
--- a/test/pivot_filtering/LakeVarese_MetaPhlAn_filtered_family_scaling.xlsx
+++ b/test/pivot_filtering/LakeVarese_MetaPhlAn_filtered_family_scaling.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="113">
   <si>
     <t xml:space="preserve">family</t>
   </si>
@@ -83,6 +83,12 @@
     <t xml:space="preserve">Comamonadaceae</t>
   </si>
   <si>
+    <t xml:space="preserve">Actinobacteria_noname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Burkholderiales_noname</t>
+  </si>
+  <si>
     <t xml:space="preserve">Pseudomonadaceae</t>
   </si>
   <si>
@@ -98,6 +104,9 @@
     <t xml:space="preserve">Sphingomonadaceae</t>
   </si>
   <si>
+    <t xml:space="preserve">Alphaproteobacteria_noname</t>
+  </si>
+  <si>
     <t xml:space="preserve">Rhodocyclaceae</t>
   </si>
   <si>
@@ -152,6 +161,9 @@
     <t xml:space="preserve">Desulfovibrionaceae</t>
   </si>
   <si>
+    <t xml:space="preserve">Chroococcales_noname</t>
+  </si>
+  <si>
     <t xml:space="preserve">Coriobacteriaceae</t>
   </si>
   <si>
@@ -176,6 +188,12 @@
     <t xml:space="preserve">Acidithiobacillaceae</t>
   </si>
   <si>
+    <t xml:space="preserve">Flavobacteriales_noname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oscillatoriales_noname</t>
+  </si>
+  <si>
     <t xml:space="preserve">Veillonellaceae</t>
   </si>
   <si>
@@ -200,6 +218,9 @@
     <t xml:space="preserve">Nocardioidaceae</t>
   </si>
   <si>
+    <t xml:space="preserve">Bacteroidales_noname</t>
+  </si>
+  <si>
     <t xml:space="preserve">Oscillospiraceae</t>
   </si>
   <si>
@@ -269,6 +290,9 @@
     <t xml:space="preserve">Methylobacteriaceae</t>
   </si>
   <si>
+    <t xml:space="preserve">Betaproteobacteria_noname</t>
+  </si>
+  <si>
     <t xml:space="preserve">Clostridiaceae</t>
   </si>
   <si>
@@ -294,6 +318,9 @@
   </si>
   <si>
     <t xml:space="preserve">Helicobacteraceae</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rhodospirillales_noname</t>
   </si>
   <si>
     <t xml:space="preserve">Sinobacteraceae</t>
@@ -728,67 +755,67 @@
         <v>22</v>
       </c>
       <c r="B2" t="n">
-        <v>19.7348292218916</v>
+        <v>15.4538272449542</v>
       </c>
       <c r="C2" t="n">
-        <v>75.9130964958003</v>
+        <v>41.2153345384156</v>
       </c>
       <c r="D2" t="n">
-        <v>30.7619789025618</v>
+        <v>2.60605869924563</v>
       </c>
       <c r="E2" t="n">
-        <v>6.47855729888277</v>
+        <v>2.92312171130139</v>
       </c>
       <c r="F2" t="n">
-        <v>79.4562200696561</v>
+        <v>2.3850027437118</v>
       </c>
       <c r="G2" t="n">
-        <v>46.854831757281</v>
+        <v>3.15400672586089</v>
       </c>
       <c r="H2" t="n">
-        <v>75.3640714550374</v>
+        <v>22.5189247141916</v>
       </c>
       <c r="I2" t="n">
-        <v>36.2731576780568</v>
+        <v>1.40983095369606</v>
       </c>
       <c r="J2" t="n">
-        <v>58.1068960186539</v>
+        <v>7.43248350901404</v>
       </c>
       <c r="K2" t="n">
-        <v>81.6597329570802</v>
+        <v>45.6577265197755</v>
       </c>
       <c r="L2" t="n">
-        <v>31.2415640008864</v>
+        <v>23.1658579701231</v>
       </c>
       <c r="M2" t="n">
-        <v>44.0047939966635</v>
+        <v>0.733432889726188</v>
       </c>
       <c r="N2" t="n">
-        <v>88.2721787360784</v>
+        <v>36.6696595020355</v>
       </c>
       <c r="O2" t="n">
-        <v>67.5224385878225</v>
+        <v>6.99042312247932</v>
       </c>
       <c r="P2" t="n">
-        <v>65.0213514075336</v>
+        <v>6.98056709795851</v>
       </c>
       <c r="Q2" t="n">
-        <v>61.3889854538296</v>
+        <v>5.98120601056716</v>
       </c>
       <c r="R2" t="n">
-        <v>71.6896673196573</v>
+        <v>26.1969046743151</v>
       </c>
       <c r="S2" t="n">
-        <v>54.364084861871</v>
+        <v>11.5881938229073</v>
       </c>
       <c r="T2" t="n">
-        <v>49.8092793556945</v>
+        <v>36.4891178721575</v>
       </c>
       <c r="U2" t="n">
-        <v>62.2983100203325</v>
+        <v>34.5530329089664</v>
       </c>
       <c r="V2" t="n">
-        <v>56.5722424469609</v>
+        <v>20.2669073101358</v>
       </c>
     </row>
     <row r="3">
@@ -796,67 +823,67 @@
         <v>23</v>
       </c>
       <c r="B3" t="n">
-        <v>17.0145522168047</v>
+        <v>6.23116083935471</v>
       </c>
       <c r="C3" t="n">
-        <v>3.27054831130322</v>
+        <v>33.2663346552947</v>
       </c>
       <c r="D3" t="n">
-        <v>3.75168729511416</v>
+        <v>83.9957691075879</v>
       </c>
       <c r="E3" t="n">
-        <v>0.249567522898642</v>
+        <v>48.0244018977011</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>81.639938234581</v>
       </c>
       <c r="G3" t="n">
-        <v>1.91340977261444</v>
+        <v>65.994260676086</v>
       </c>
       <c r="H3" t="n">
-        <v>0</v>
+        <v>57.9137359071011</v>
       </c>
       <c r="I3" t="n">
-        <v>0</v>
+        <v>67.8283480909948</v>
       </c>
       <c r="J3" t="n">
-        <v>4.0680616300266</v>
+        <v>59.0810877613969</v>
       </c>
       <c r="K3" t="n">
-        <v>0.902163324545905</v>
+        <v>32.6564840742851</v>
       </c>
       <c r="L3" t="n">
-        <v>12.0375684067988</v>
+        <v>12.2408593806696</v>
       </c>
       <c r="M3" t="n">
-        <v>0</v>
+        <v>76.5268751569057</v>
       </c>
       <c r="N3" t="n">
-        <v>2.07398563191264</v>
+        <v>37.9792909131016</v>
       </c>
       <c r="O3" t="n">
-        <v>0.958563771627465</v>
+        <v>56.1879193472689</v>
       </c>
       <c r="P3" t="n">
-        <v>0.556506889219707</v>
+        <v>82.2811635622854</v>
       </c>
       <c r="Q3" t="n">
-        <v>0</v>
+        <v>63.4980570430531</v>
       </c>
       <c r="R3" t="n">
-        <v>0.924770497560249</v>
+        <v>58.1887581749553</v>
       </c>
       <c r="S3" t="n">
-        <v>0</v>
+        <v>71.4891223368351</v>
       </c>
       <c r="T3" t="n">
-        <v>0.11170068043944</v>
+        <v>22.8374470734807</v>
       </c>
       <c r="U3" t="n">
-        <v>12.1690349283724</v>
+        <v>38.2487810088918</v>
       </c>
       <c r="V3" t="n">
-        <v>2.09471993260427</v>
+        <v>52.4084010268175</v>
       </c>
     </row>
     <row r="4">
@@ -864,67 +891,67 @@
         <v>24</v>
       </c>
       <c r="B4" t="n">
-        <v>6.63697502989491</v>
+        <v>12.4946934633559</v>
       </c>
       <c r="C4" t="n">
-        <v>3.76476056859292</v>
+        <v>8.47110324267464</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>0.550401226874093</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>0.077992832409256</v>
       </c>
       <c r="F4" t="n">
-        <v>0.382292120156726</v>
+        <v>0.135353045520093</v>
       </c>
       <c r="G4" t="n">
         <v>0</v>
       </c>
       <c r="H4" t="n">
-        <v>0</v>
+        <v>0.0237127743946042</v>
       </c>
       <c r="I4" t="n">
-        <v>0</v>
+        <v>0.0351327649486015</v>
       </c>
       <c r="J4" t="n">
-        <v>0</v>
+        <v>0.841011962079744</v>
       </c>
       <c r="K4" t="n">
-        <v>0.054752992632941</v>
+        <v>0.158818597657786</v>
       </c>
       <c r="L4" t="n">
-        <v>6.79238471912853</v>
+        <v>9.67401789370424</v>
       </c>
       <c r="M4" t="n">
         <v>0</v>
       </c>
       <c r="N4" t="n">
-        <v>1.09781107255903</v>
+        <v>0.581056902720512</v>
       </c>
       <c r="O4" t="n">
-        <v>1.69398191419063</v>
+        <v>0.343700537193873</v>
       </c>
       <c r="P4" t="n">
-        <v>0</v>
+        <v>0.248319144692512</v>
       </c>
       <c r="Q4" t="n">
-        <v>0</v>
+        <v>0.828896345363785</v>
       </c>
       <c r="R4" t="n">
-        <v>0</v>
+        <v>0.133757901898336</v>
       </c>
       <c r="S4" t="n">
         <v>0</v>
       </c>
       <c r="T4" t="n">
-        <v>0</v>
+        <v>0.34009120955523</v>
       </c>
       <c r="U4" t="n">
-        <v>4.24114705689445</v>
+        <v>1.43891246929849</v>
       </c>
       <c r="V4" t="n">
-        <v>1.27188203289955</v>
+        <v>0.809509900075121</v>
       </c>
     </row>
     <row r="5">
@@ -932,22 +959,22 @@
         <v>25</v>
       </c>
       <c r="B5" t="n">
-        <v>7.00494237282576</v>
+        <v>13.3236496577876</v>
       </c>
       <c r="C5" t="n">
-        <v>2.59910233035806</v>
+        <v>1.77567177465709</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>0.317831220912363</v>
       </c>
       <c r="E5" t="n">
-        <v>54.234920890517</v>
+        <v>0.112604737592818</v>
       </c>
       <c r="F5" t="n">
         <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>0</v>
+        <v>0.12880010589764</v>
       </c>
       <c r="H5" t="n">
         <v>0</v>
@@ -956,43 +983,43 @@
         <v>0</v>
       </c>
       <c r="J5" t="n">
-        <v>2.58810040644384</v>
+        <v>0.520347894148725</v>
       </c>
       <c r="K5" t="n">
-        <v>0</v>
+        <v>0.504419067472801</v>
       </c>
       <c r="L5" t="n">
-        <v>4.06971109476468</v>
+        <v>8.92594877803266</v>
       </c>
       <c r="M5" t="n">
         <v>0</v>
       </c>
       <c r="N5" t="n">
-        <v>0.604642560594297</v>
+        <v>0.861566441695482</v>
       </c>
       <c r="O5" t="n">
-        <v>0.127894493492165</v>
+        <v>0.0992376237247462</v>
       </c>
       <c r="P5" t="n">
-        <v>0</v>
+        <v>0.0597455081535606</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.421139484915625</v>
+        <v>0</v>
       </c>
       <c r="R5" t="n">
-        <v>0.890802576306704</v>
+        <v>0.337930492300694</v>
       </c>
       <c r="S5" t="n">
-        <v>0.53974604491175</v>
+        <v>0</v>
       </c>
       <c r="T5" t="n">
-        <v>24.0507936091468</v>
+        <v>0.0818293166991771</v>
       </c>
       <c r="U5" t="n">
-        <v>4.05940095353743</v>
+        <v>6.7494136552529</v>
       </c>
       <c r="V5" t="n">
-        <v>2.27748279422991</v>
+        <v>0.750429766940683</v>
       </c>
     </row>
     <row r="6">
@@ -1000,10 +1027,10 @@
         <v>26</v>
       </c>
       <c r="B6" t="n">
-        <v>7.14336942242143</v>
+        <v>5.19724110038382</v>
       </c>
       <c r="C6" t="n">
-        <v>1.42962884869592</v>
+        <v>2.04399337471601</v>
       </c>
       <c r="D6" t="n">
         <v>0</v>
@@ -1012,7 +1039,7 @@
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>0.0619013931214628</v>
+        <v>0.0114750960299128</v>
       </c>
       <c r="G6" t="n">
         <v>0</v>
@@ -1027,28 +1054,28 @@
         <v>0</v>
       </c>
       <c r="K6" t="n">
-        <v>0</v>
+        <v>0.030613584850786</v>
       </c>
       <c r="L6" t="n">
-        <v>5.77595401995946</v>
+        <v>5.03660507128584</v>
       </c>
       <c r="M6" t="n">
         <v>0</v>
       </c>
       <c r="N6" t="n">
-        <v>0.293627797567559</v>
+        <v>0.456048086777887</v>
       </c>
       <c r="O6" t="n">
-        <v>0</v>
+        <v>0.175373558622564</v>
       </c>
       <c r="P6" t="n">
-        <v>0.98614512245482</v>
+        <v>0</v>
       </c>
       <c r="Q6" t="n">
         <v>0</v>
       </c>
       <c r="R6" t="n">
-        <v>0.0625984173302637</v>
+        <v>0</v>
       </c>
       <c r="S6" t="n">
         <v>0</v>
@@ -1057,10 +1084,10 @@
         <v>0</v>
       </c>
       <c r="U6" t="n">
-        <v>5.36961805234708</v>
+        <v>2.35230287596584</v>
       </c>
       <c r="V6" t="n">
-        <v>1.56201772657302</v>
+        <v>0.455649522720784</v>
       </c>
     </row>
     <row r="7">
@@ -1068,67 +1095,67 @@
         <v>27</v>
       </c>
       <c r="B7" t="n">
-        <v>1.29944406603523</v>
+        <v>5.48538667719633</v>
       </c>
       <c r="C7" t="n">
-        <v>8.6338958759246</v>
+        <v>1.41112504943346</v>
       </c>
       <c r="D7" t="n">
         <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
+        <v>24.4707683287949</v>
       </c>
       <c r="F7" t="n">
-        <v>3.06683989986939</v>
+        <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>46.4112976345838</v>
+        <v>0</v>
       </c>
       <c r="H7" t="n">
-        <v>23.2363759171448</v>
+        <v>0</v>
       </c>
       <c r="I7" t="n">
-        <v>52.8671778509675</v>
+        <v>0</v>
       </c>
       <c r="J7" t="n">
-        <v>2.0535559005211</v>
+        <v>0.331045278763318</v>
       </c>
       <c r="K7" t="n">
-        <v>16.7923010244766</v>
+        <v>0</v>
       </c>
       <c r="L7" t="n">
-        <v>3.1974988879046</v>
+        <v>3.01772181437772</v>
       </c>
       <c r="M7" t="n">
-        <v>13.2479327395041</v>
+        <v>0</v>
       </c>
       <c r="N7" t="n">
-        <v>3.64818029271751</v>
+        <v>0.251178085042209</v>
       </c>
       <c r="O7" t="n">
-        <v>3.14953832965227</v>
+        <v>0.0132405855482039</v>
       </c>
       <c r="P7" t="n">
-        <v>28.5128215645021</v>
+        <v>0</v>
       </c>
       <c r="Q7" t="n">
-        <v>4.46520939700197</v>
+        <v>0.0410321493317228</v>
       </c>
       <c r="R7" t="n">
-        <v>0.166336065638834</v>
+        <v>0.325517903034573</v>
       </c>
       <c r="S7" t="n">
-        <v>0.360815891474687</v>
+        <v>0.115051725775887</v>
       </c>
       <c r="T7" t="n">
-        <v>0.151207246031613</v>
+        <v>17.6190511943787</v>
       </c>
       <c r="U7" t="n">
-        <v>0.430294906651969</v>
+        <v>2.25149951407172</v>
       </c>
       <c r="V7" t="n">
-        <v>0.25418646504559</v>
+        <v>0.815904243752781</v>
       </c>
     </row>
     <row r="8">
@@ -1136,19 +1163,19 @@
         <v>28</v>
       </c>
       <c r="B8" t="n">
-        <v>7.11107628560461</v>
+        <v>5.59378526967603</v>
       </c>
       <c r="C8" t="n">
-        <v>0.192789595407258</v>
+        <v>0.776185322226083</v>
       </c>
       <c r="D8" t="n">
-        <v>3.30436066096736</v>
+        <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>0.436178456769623</v>
+        <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>0</v>
+        <v>0.00185806715075101</v>
       </c>
       <c r="G8" t="n">
         <v>0</v>
@@ -1166,37 +1193,37 @@
         <v>0</v>
       </c>
       <c r="L8" t="n">
-        <v>1.14741838689813</v>
+        <v>4.28291395605373</v>
       </c>
       <c r="M8" t="n">
         <v>0</v>
       </c>
       <c r="N8" t="n">
-        <v>1.13174214504101</v>
+        <v>0.1219776322654</v>
       </c>
       <c r="O8" t="n">
         <v>0</v>
       </c>
       <c r="P8" t="n">
-        <v>0</v>
+        <v>0.105870641667758</v>
       </c>
       <c r="Q8" t="n">
         <v>0</v>
       </c>
       <c r="R8" t="n">
-        <v>0</v>
+        <v>0.0228747716773719</v>
       </c>
       <c r="S8" t="n">
         <v>0</v>
       </c>
       <c r="T8" t="n">
-        <v>0.0455329908519958</v>
+        <v>0</v>
       </c>
       <c r="U8" t="n">
-        <v>0.0524347745105393</v>
+        <v>2.97819618559114</v>
       </c>
       <c r="V8" t="n">
-        <v>0.0111171662734225</v>
+        <v>0.55959012957502</v>
       </c>
     </row>
     <row r="9">
@@ -1204,10 +1231,10 @@
         <v>29</v>
       </c>
       <c r="B9" t="n">
-        <v>4.68998914060296</v>
+        <v>1.01756057198171</v>
       </c>
       <c r="C9" t="n">
-        <v>0.0736139239059836</v>
+        <v>4.68758255587382</v>
       </c>
       <c r="D9" t="n">
         <v>0</v>
@@ -1216,55 +1243,55 @@
         <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>0.547929364388333</v>
+        <v>0.0920559972435268</v>
       </c>
       <c r="G9" t="n">
-        <v>0</v>
+        <v>3.1241504751036</v>
       </c>
       <c r="H9" t="n">
-        <v>0</v>
+        <v>6.94307233946372</v>
       </c>
       <c r="I9" t="n">
-        <v>0</v>
+        <v>2.05479171210774</v>
       </c>
       <c r="J9" t="n">
-        <v>0.285348053771683</v>
+        <v>0.262671410989871</v>
       </c>
       <c r="K9" t="n">
-        <v>0</v>
+        <v>9.38893944480899</v>
       </c>
       <c r="L9" t="n">
-        <v>1.4177651047602</v>
+        <v>2.37096981107356</v>
       </c>
       <c r="M9" t="n">
-        <v>0</v>
+        <v>0.220804796694864</v>
       </c>
       <c r="N9" t="n">
-        <v>0.0944242265449354</v>
+        <v>1.51551180736077</v>
       </c>
       <c r="O9" t="n">
-        <v>0</v>
+        <v>0.326063543100571</v>
       </c>
       <c r="P9" t="n">
-        <v>0</v>
+        <v>3.06108162587443</v>
       </c>
       <c r="Q9" t="n">
-        <v>0.287216709876569</v>
+        <v>0.435050963725009</v>
       </c>
       <c r="R9" t="n">
-        <v>0</v>
+        <v>0.0607826792668951</v>
       </c>
       <c r="S9" t="n">
-        <v>0</v>
+        <v>0.076911153667305</v>
       </c>
       <c r="T9" t="n">
-        <v>0</v>
+        <v>0.110770906444384</v>
       </c>
       <c r="U9" t="n">
-        <v>0.499380530428295</v>
+        <v>0.238658064163435</v>
       </c>
       <c r="V9" t="n">
-        <v>0.978338564639758</v>
+        <v>0.091061858320357</v>
       </c>
     </row>
     <row r="10">
@@ -1272,67 +1299,67 @@
         <v>30</v>
       </c>
       <c r="B10" t="n">
-        <v>3.13665151279874</v>
+        <v>2.50467510337618</v>
       </c>
       <c r="C10" t="n">
-        <v>0.0930771947233893</v>
+        <v>3.12023177286387</v>
       </c>
       <c r="D10" t="n">
-        <v>0</v>
+        <v>6.64505035201638</v>
       </c>
       <c r="E10" t="n">
-        <v>0</v>
+        <v>4.9580090989956</v>
       </c>
       <c r="F10" t="n">
-        <v>0</v>
+        <v>11.5676522760046</v>
       </c>
       <c r="G10" t="n">
-        <v>0</v>
+        <v>23.9777610953642</v>
       </c>
       <c r="H10" t="n">
-        <v>0</v>
+        <v>11.4326576209416</v>
       </c>
       <c r="I10" t="n">
-        <v>0</v>
+        <v>23.1622428685138</v>
       </c>
       <c r="J10" t="n">
-        <v>0</v>
+        <v>22.6484343218484</v>
       </c>
       <c r="K10" t="n">
-        <v>0</v>
+        <v>9.81644950623718</v>
       </c>
       <c r="L10" t="n">
-        <v>2.20204418653148</v>
+        <v>3.22749204214542</v>
       </c>
       <c r="M10" t="n">
-        <v>0</v>
+        <v>3.62180295041463</v>
       </c>
       <c r="N10" t="n">
-        <v>0</v>
+        <v>16.8949174652702</v>
       </c>
       <c r="O10" t="n">
-        <v>0</v>
+        <v>24.8143467548085</v>
       </c>
       <c r="P10" t="n">
-        <v>0</v>
+        <v>4.67399017831883</v>
       </c>
       <c r="Q10" t="n">
-        <v>0.04251184258472</v>
+        <v>20.8326404524759</v>
       </c>
       <c r="R10" t="n">
-        <v>0.00812930911547369</v>
+        <v>5.09370254635117</v>
       </c>
       <c r="S10" t="n">
-        <v>0</v>
+        <v>7.17307759616394</v>
       </c>
       <c r="T10" t="n">
-        <v>0</v>
+        <v>3.09682017922563</v>
       </c>
       <c r="U10" t="n">
-        <v>0.26525400789022</v>
+        <v>4.60428475085612</v>
       </c>
       <c r="V10" t="n">
-        <v>1.1339509598891</v>
+        <v>10.7641620953113</v>
       </c>
     </row>
     <row r="11">
@@ -1340,16 +1367,16 @@
         <v>31</v>
       </c>
       <c r="B11" t="n">
-        <v>2.25356893829772</v>
+        <v>5.5684973610778</v>
       </c>
       <c r="C11" t="n">
-        <v>0.134860561146741</v>
+        <v>0.104670841225341</v>
       </c>
       <c r="D11" t="n">
-        <v>0</v>
+        <v>0.279935106685931</v>
       </c>
       <c r="E11" t="n">
-        <v>0</v>
+        <v>0.196803494692421</v>
       </c>
       <c r="F11" t="n">
         <v>0</v>
@@ -1370,13 +1397,13 @@
         <v>0</v>
       </c>
       <c r="L11" t="n">
-        <v>1.44135459481886</v>
+        <v>0.850819484659461</v>
       </c>
       <c r="M11" t="n">
         <v>0</v>
       </c>
       <c r="N11" t="n">
-        <v>0</v>
+        <v>0.470143591072314</v>
       </c>
       <c r="O11" t="n">
         <v>0</v>
@@ -1394,13 +1421,13 @@
         <v>0</v>
       </c>
       <c r="T11" t="n">
-        <v>0</v>
+        <v>0.0333564085198995</v>
       </c>
       <c r="U11" t="n">
-        <v>0.246483300774491</v>
+        <v>0.0290823376853333</v>
       </c>
       <c r="V11" t="n">
-        <v>0.38147522561842</v>
+        <v>0.00398270545181342</v>
       </c>
     </row>
     <row r="12">
@@ -1408,10 +1435,10 @@
         <v>32</v>
       </c>
       <c r="B12" t="n">
-        <v>1.56442741118509</v>
+        <v>3.67260750750203</v>
       </c>
       <c r="C12" t="n">
-        <v>0.741318385934543</v>
+        <v>0.0399670496992364</v>
       </c>
       <c r="D12" t="n">
         <v>0</v>
@@ -1420,55 +1447,55 @@
         <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>0</v>
+        <v>0.0164469570321971</v>
       </c>
       <c r="G12" t="n">
-        <v>0.544161669971372</v>
+        <v>0</v>
       </c>
       <c r="H12" t="n">
-        <v>0.00552270013846915</v>
+        <v>0</v>
       </c>
       <c r="I12" t="n">
-        <v>0.0630403458213256</v>
+        <v>0</v>
       </c>
       <c r="J12" t="n">
-        <v>0</v>
+        <v>0.0364990190373693</v>
       </c>
       <c r="K12" t="n">
-        <v>0.0350590870828371</v>
+        <v>0</v>
       </c>
       <c r="L12" t="n">
-        <v>4.27510164034753</v>
+        <v>1.05128363775065</v>
       </c>
       <c r="M12" t="n">
         <v>0</v>
       </c>
       <c r="N12" t="n">
-        <v>0.282189004502309</v>
+        <v>0.0392253174864785</v>
       </c>
       <c r="O12" t="n">
         <v>0</v>
       </c>
       <c r="P12" t="n">
-        <v>0.760745849735683</v>
+        <v>0</v>
       </c>
       <c r="Q12" t="n">
-        <v>0</v>
+        <v>0.027983885036528</v>
       </c>
       <c r="R12" t="n">
-        <v>0.274507882555844</v>
+        <v>0</v>
       </c>
       <c r="S12" t="n">
-        <v>0.137974195400735</v>
+        <v>0</v>
       </c>
       <c r="T12" t="n">
-        <v>0.155662154500325</v>
+        <v>0</v>
       </c>
       <c r="U12" t="n">
-        <v>1.4202866410182</v>
+        <v>0.276975601687338</v>
       </c>
       <c r="V12" t="n">
-        <v>0.430552766177223</v>
+        <v>0.350488086557198</v>
       </c>
     </row>
     <row r="13">
@@ -1476,10 +1503,10 @@
         <v>33</v>
       </c>
       <c r="B13" t="n">
-        <v>2.01524272503051</v>
+        <v>2.45622954530791</v>
       </c>
       <c r="C13" t="n">
-        <v>0</v>
+        <v>0.0505342015476074</v>
       </c>
       <c r="D13" t="n">
         <v>0</v>
@@ -1506,7 +1533,7 @@
         <v>0</v>
       </c>
       <c r="L13" t="n">
-        <v>0.667897004447837</v>
+        <v>1.63283255818038</v>
       </c>
       <c r="M13" t="n">
         <v>0</v>
@@ -1521,10 +1548,10 @@
         <v>0</v>
       </c>
       <c r="Q13" t="n">
-        <v>0</v>
+        <v>0.00414198225476864</v>
       </c>
       <c r="R13" t="n">
-        <v>0</v>
+        <v>0.00297061967126343</v>
       </c>
       <c r="S13" t="n">
         <v>0</v>
@@ -1533,10 +1560,10 @@
         <v>0</v>
       </c>
       <c r="U13" t="n">
-        <v>0.111392188559363</v>
+        <v>0.147120049659046</v>
       </c>
       <c r="V13" t="n">
-        <v>0.439519123900259</v>
+        <v>0.406235956084968</v>
       </c>
     </row>
     <row r="14">
@@ -1544,10 +1571,10 @@
         <v>34</v>
       </c>
       <c r="B14" t="n">
-        <v>1.57210695601456</v>
+        <v>1.76471073884012</v>
       </c>
       <c r="C14" t="n">
-        <v>0</v>
+        <v>0.0732195549948205</v>
       </c>
       <c r="D14" t="n">
         <v>0</v>
@@ -1574,7 +1601,7 @@
         <v>0</v>
       </c>
       <c r="L14" t="n">
-        <v>0.463432070708033</v>
+        <v>1.06877542453414</v>
       </c>
       <c r="M14" t="n">
         <v>0</v>
@@ -1583,7 +1610,7 @@
         <v>0</v>
       </c>
       <c r="O14" t="n">
-        <v>1.30851247492216</v>
+        <v>0</v>
       </c>
       <c r="P14" t="n">
         <v>0</v>
@@ -1592,7 +1619,7 @@
         <v>0</v>
       </c>
       <c r="R14" t="n">
-        <v>0.0901614283716173</v>
+        <v>0</v>
       </c>
       <c r="S14" t="n">
         <v>0</v>
@@ -1601,10 +1628,10 @@
         <v>0</v>
       </c>
       <c r="U14" t="n">
-        <v>0</v>
+        <v>0.13670909532525</v>
       </c>
       <c r="V14" t="n">
-        <v>0.128294333401582</v>
+        <v>0.136662835063859</v>
       </c>
     </row>
     <row r="15">
@@ -1612,10 +1639,10 @@
         <v>35</v>
       </c>
       <c r="B15" t="n">
-        <v>1.43119381648257</v>
+        <v>1.22506208074538</v>
       </c>
       <c r="C15" t="n">
-        <v>0.1758329579527</v>
+        <v>0.40248240008838</v>
       </c>
       <c r="D15" t="n">
         <v>0</v>
@@ -1627,52 +1654,52 @@
         <v>0</v>
       </c>
       <c r="G15" t="n">
-        <v>0</v>
+        <v>0.0366299376750765</v>
       </c>
       <c r="H15" t="n">
-        <v>0</v>
+        <v>0.00165019307258949</v>
       </c>
       <c r="I15" t="n">
-        <v>0</v>
+        <v>0.00245019283017573</v>
       </c>
       <c r="J15" t="n">
         <v>0</v>
       </c>
       <c r="K15" t="n">
-        <v>0</v>
+        <v>0.0196022954287947</v>
       </c>
       <c r="L15" t="n">
-        <v>0.508868722650212</v>
+        <v>3.17002047033628</v>
       </c>
       <c r="M15" t="n">
         <v>0</v>
       </c>
       <c r="N15" t="n">
-        <v>0</v>
+        <v>0.117225776665788</v>
       </c>
       <c r="O15" t="n">
         <v>0</v>
       </c>
       <c r="P15" t="n">
-        <v>0</v>
+        <v>0.0816722097221454</v>
       </c>
       <c r="Q15" t="n">
         <v>0</v>
       </c>
       <c r="R15" t="n">
-        <v>0</v>
+        <v>0.100310924858926</v>
       </c>
       <c r="S15" t="n">
-        <v>0</v>
+        <v>0.0294104411566173</v>
       </c>
       <c r="T15" t="n">
-        <v>0</v>
+        <v>0.114034468622501</v>
       </c>
       <c r="U15" t="n">
-        <v>0</v>
+        <v>0.78774546261769</v>
       </c>
       <c r="V15" t="n">
-        <v>0</v>
+        <v>0.15424477847802</v>
       </c>
     </row>
     <row r="16">
@@ -1680,52 +1707,52 @@
         <v>36</v>
       </c>
       <c r="B16" t="n">
-        <v>1.3144517188969</v>
+        <v>1.57808373100719</v>
       </c>
       <c r="C16" t="n">
-        <v>0.305864563650425</v>
+        <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>1.26567964366232</v>
+        <v>0</v>
       </c>
       <c r="E16" t="n">
-        <v>0.158565618545692</v>
+        <v>0</v>
       </c>
       <c r="F16" t="n">
-        <v>6.48298051806704</v>
+        <v>0</v>
       </c>
       <c r="G16" t="n">
-        <v>2.38919821991801</v>
+        <v>0</v>
       </c>
       <c r="H16" t="n">
-        <v>0.105801546289097</v>
+        <v>0</v>
       </c>
       <c r="I16" t="n">
-        <v>9.31762041992589</v>
+        <v>0</v>
       </c>
       <c r="J16" t="n">
-        <v>2.75331886195724</v>
+        <v>0</v>
       </c>
       <c r="K16" t="n">
         <v>0</v>
       </c>
       <c r="L16" t="n">
-        <v>5.14927396640465</v>
+        <v>0.49525072250769</v>
       </c>
       <c r="M16" t="n">
-        <v>9.34648671111352</v>
+        <v>0</v>
       </c>
       <c r="N16" t="n">
-        <v>0.953369218231943</v>
+        <v>0</v>
       </c>
       <c r="O16" t="n">
-        <v>2.15614836158125</v>
+        <v>0</v>
       </c>
       <c r="P16" t="n">
         <v>0</v>
       </c>
       <c r="Q16" t="n">
-        <v>1.79376939733704</v>
+        <v>0</v>
       </c>
       <c r="R16" t="n">
         <v>0</v>
@@ -1734,13 +1761,13 @@
         <v>0</v>
       </c>
       <c r="T16" t="n">
-        <v>0.0357895867471119</v>
+        <v>0</v>
       </c>
       <c r="U16" t="n">
-        <v>0.723288251023058</v>
+        <v>0.0617823815098235</v>
       </c>
       <c r="V16" t="n">
-        <v>0.221030494275358</v>
+        <v>0.157456960513277</v>
       </c>
     </row>
     <row r="17">
@@ -1748,10 +1775,10 @@
         <v>37</v>
       </c>
       <c r="B17" t="n">
-        <v>1.49304669280402</v>
+        <v>1.23107573091586</v>
       </c>
       <c r="C17" t="n">
-        <v>0.0480130875751345</v>
+        <v>0</v>
       </c>
       <c r="D17" t="n">
         <v>0</v>
@@ -1760,7 +1787,7 @@
         <v>0</v>
       </c>
       <c r="F17" t="n">
-        <v>0.242843926861123</v>
+        <v>0</v>
       </c>
       <c r="G17" t="n">
         <v>0</v>
@@ -1778,16 +1805,16 @@
         <v>0</v>
       </c>
       <c r="L17" t="n">
-        <v>1.33176487499068</v>
+        <v>0.343638414789916</v>
       </c>
       <c r="M17" t="n">
         <v>0</v>
       </c>
       <c r="N17" t="n">
-        <v>0.250642017311831</v>
+        <v>0</v>
       </c>
       <c r="O17" t="n">
-        <v>0</v>
+        <v>0.135466906291476</v>
       </c>
       <c r="P17" t="n">
         <v>0</v>
@@ -1796,7 +1823,7 @@
         <v>0</v>
       </c>
       <c r="R17" t="n">
-        <v>0</v>
+        <v>0.0329468727176489</v>
       </c>
       <c r="S17" t="n">
         <v>0</v>
@@ -1805,10 +1832,10 @@
         <v>0</v>
       </c>
       <c r="U17" t="n">
-        <v>0.274150163482713</v>
+        <v>0</v>
       </c>
       <c r="V17" t="n">
-        <v>0.172986459123884</v>
+        <v>0.0459612214577362</v>
       </c>
     </row>
     <row r="18">
@@ -1816,10 +1843,10 @@
         <v>38</v>
       </c>
       <c r="B18" t="n">
-        <v>1.4316884312343</v>
+        <v>1.12073034660131</v>
       </c>
       <c r="C18" t="n">
-        <v>0.0186523012000139</v>
+        <v>0.0954646104483514</v>
       </c>
       <c r="D18" t="n">
         <v>0</v>
@@ -1840,19 +1867,19 @@
         <v>0</v>
       </c>
       <c r="J18" t="n">
-        <v>0.0833338701054435</v>
+        <v>0</v>
       </c>
       <c r="K18" t="n">
         <v>0</v>
       </c>
       <c r="L18" t="n">
-        <v>1.27596953756977</v>
+        <v>0.3773300387272</v>
       </c>
       <c r="M18" t="n">
         <v>0</v>
       </c>
       <c r="N18" t="n">
-        <v>0.322694372788099</v>
+        <v>0</v>
       </c>
       <c r="O18" t="n">
         <v>0</v>
@@ -1864,7 +1891,7 @@
         <v>0</v>
       </c>
       <c r="R18" t="n">
-        <v>0.0194884447482063</v>
+        <v>0</v>
       </c>
       <c r="S18" t="n">
         <v>0</v>
@@ -1876,7 +1903,7 @@
         <v>0</v>
       </c>
       <c r="V18" t="n">
-        <v>0.136646174395937</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
@@ -1884,52 +1911,52 @@
         <v>39</v>
       </c>
       <c r="B19" t="n">
-        <v>1.31994454587662</v>
+        <v>1.02931267138266</v>
       </c>
       <c r="C19" t="n">
-        <v>0.0245133997984372</v>
+        <v>0.166062391026247</v>
       </c>
       <c r="D19" t="n">
-        <v>0</v>
+        <v>0.107224423248974</v>
       </c>
       <c r="E19" t="n">
-        <v>0</v>
+        <v>0.0715447252919686</v>
       </c>
       <c r="F19" t="n">
-        <v>0</v>
+        <v>0.194596801980577</v>
       </c>
       <c r="G19" t="n">
-        <v>0</v>
+        <v>0.160827538429167</v>
       </c>
       <c r="H19" t="n">
-        <v>0</v>
+        <v>0.0316136988027599</v>
       </c>
       <c r="I19" t="n">
-        <v>0</v>
+        <v>0.362148501087036</v>
       </c>
       <c r="J19" t="n">
-        <v>0</v>
+        <v>0.352178457957641</v>
       </c>
       <c r="K19" t="n">
         <v>0</v>
       </c>
       <c r="L19" t="n">
-        <v>0.990813030219049</v>
+        <v>3.81822591697387</v>
       </c>
       <c r="M19" t="n">
-        <v>0</v>
+        <v>0.155778953489458</v>
       </c>
       <c r="N19" t="n">
-        <v>0</v>
+        <v>0.396044655437949</v>
       </c>
       <c r="O19" t="n">
-        <v>0</v>
+        <v>0.223220453489541</v>
       </c>
       <c r="P19" t="n">
         <v>0</v>
       </c>
       <c r="Q19" t="n">
-        <v>0</v>
+        <v>0.174769206912417</v>
       </c>
       <c r="R19" t="n">
         <v>0</v>
@@ -1938,13 +1965,13 @@
         <v>0</v>
       </c>
       <c r="T19" t="n">
-        <v>0</v>
+        <v>0.0262186176211335</v>
       </c>
       <c r="U19" t="n">
-        <v>0.231263808518495</v>
+        <v>0.401163414097618</v>
       </c>
       <c r="V19" t="n">
-        <v>0.300414882589596</v>
+        <v>0.0791837895482401</v>
       </c>
     </row>
     <row r="20">
@@ -1952,67 +1979,67 @@
         <v>40</v>
       </c>
       <c r="B20" t="n">
-        <v>0.653555297343515</v>
+        <v>1.16916571204217</v>
       </c>
       <c r="C20" t="n">
-        <v>0.823613370972153</v>
+        <v>0.0260676425804985</v>
       </c>
       <c r="D20" t="n">
-        <v>54.6584819462399</v>
+        <v>0</v>
       </c>
       <c r="E20" t="n">
-        <v>33.9300007715816</v>
+        <v>0</v>
       </c>
       <c r="F20" t="n">
-        <v>0.448615041358293</v>
+        <v>0.00728934036063858</v>
       </c>
       <c r="G20" t="n">
-        <v>0.170041232026018</v>
+        <v>0</v>
       </c>
       <c r="H20" t="n">
-        <v>0.0521142067611908</v>
+        <v>0</v>
       </c>
       <c r="I20" t="n">
         <v>0</v>
       </c>
       <c r="J20" t="n">
-        <v>3.4373007233541</v>
+        <v>0</v>
       </c>
       <c r="K20" t="n">
-        <v>0.185276542859197</v>
+        <v>0</v>
       </c>
       <c r="L20" t="n">
-        <v>0.473259890570901</v>
+        <v>0.987513811496676</v>
       </c>
       <c r="M20" t="n">
         <v>0</v>
       </c>
       <c r="N20" t="n">
-        <v>0.350291966162364</v>
+        <v>0.104120659117385</v>
       </c>
       <c r="O20" t="n">
-        <v>5.09891235109569</v>
+        <v>0</v>
       </c>
       <c r="P20" t="n">
-        <v>3.08567689228655</v>
+        <v>0</v>
       </c>
       <c r="Q20" t="n">
-        <v>3.14472455257856</v>
+        <v>0</v>
       </c>
       <c r="R20" t="n">
-        <v>20.27493487657</v>
+        <v>0</v>
       </c>
       <c r="S20" t="n">
-        <v>37.0437961340953</v>
+        <v>0</v>
       </c>
       <c r="T20" t="n">
-        <v>21.7196329319406</v>
+        <v>0</v>
       </c>
       <c r="U20" t="n">
-        <v>2.18185916244235</v>
+        <v>0.152054198865507</v>
       </c>
       <c r="V20" t="n">
-        <v>23.1354654642995</v>
+        <v>0.0619720976459309</v>
       </c>
     </row>
     <row r="21">
@@ -2020,10 +2047,10 @@
         <v>41</v>
       </c>
       <c r="B21" t="n">
-        <v>1.19200853548867</v>
+        <v>1.1211176664428</v>
       </c>
       <c r="C21" t="n">
-        <v>0.0247898667134572</v>
+        <v>0.0101268538546889</v>
       </c>
       <c r="D21" t="n">
         <v>0</v>
@@ -2044,19 +2071,19 @@
         <v>0</v>
       </c>
       <c r="J21" t="n">
-        <v>0</v>
+        <v>0.0106592789795929</v>
       </c>
       <c r="K21" t="n">
         <v>0</v>
       </c>
       <c r="L21" t="n">
-        <v>1.39798695758465</v>
+        <v>0.946141143276507</v>
       </c>
       <c r="M21" t="n">
         <v>0</v>
       </c>
       <c r="N21" t="n">
-        <v>0</v>
+        <v>0.134052347441676</v>
       </c>
       <c r="O21" t="n">
         <v>0</v>
@@ -2068,7 +2095,7 @@
         <v>0</v>
       </c>
       <c r="R21" t="n">
-        <v>0</v>
+        <v>0.00712148554188404</v>
       </c>
       <c r="S21" t="n">
         <v>0</v>
@@ -2077,10 +2104,10 @@
         <v>0</v>
       </c>
       <c r="U21" t="n">
-        <v>0.128894604653758</v>
+        <v>0</v>
       </c>
       <c r="V21" t="n">
-        <v>0</v>
+        <v>0.0489532539454051</v>
       </c>
     </row>
     <row r="22">
@@ -2088,10 +2115,10 @@
         <v>42</v>
       </c>
       <c r="B22" t="n">
-        <v>1.05455769921878</v>
+        <v>1.03361396014866</v>
       </c>
       <c r="C22" t="n">
-        <v>0.157438692540038</v>
+        <v>0.0133090075363006</v>
       </c>
       <c r="D22" t="n">
         <v>0</v>
@@ -2118,7 +2145,7 @@
         <v>0</v>
       </c>
       <c r="L22" t="n">
-        <v>1.03344562275437</v>
+        <v>0.734695418332786</v>
       </c>
       <c r="M22" t="n">
         <v>0</v>
@@ -2127,7 +2154,7 @@
         <v>0</v>
       </c>
       <c r="O22" t="n">
-        <v>0.0675687742964811</v>
+        <v>0</v>
       </c>
       <c r="P22" t="n">
         <v>0</v>
@@ -2145,10 +2172,10 @@
         <v>0</v>
       </c>
       <c r="U22" t="n">
-        <v>0.249509080782528</v>
+        <v>0.128267781000551</v>
       </c>
       <c r="V22" t="n">
-        <v>0.558679504107346</v>
+        <v>0.107623108377521</v>
       </c>
     </row>
     <row r="23">
@@ -2156,67 +2183,67 @@
         <v>43</v>
       </c>
       <c r="B23" t="n">
-        <v>1.00341713712556</v>
+        <v>0.51178201476239</v>
       </c>
       <c r="C23" t="n">
-        <v>0.0809863749731827</v>
+        <v>0.447162639674532</v>
       </c>
       <c r="D23" t="n">
-        <v>0</v>
+        <v>4.63049574329225</v>
       </c>
       <c r="E23" t="n">
-        <v>0</v>
+        <v>15.3091988453953</v>
       </c>
       <c r="F23" t="n">
-        <v>0</v>
+        <v>0.0134658822628604</v>
       </c>
       <c r="G23" t="n">
-        <v>0</v>
+        <v>0.0114462301830887</v>
       </c>
       <c r="H23" t="n">
-        <v>0</v>
+        <v>0.0155718219031627</v>
       </c>
       <c r="I23" t="n">
         <v>0</v>
       </c>
       <c r="J23" t="n">
-        <v>0</v>
+        <v>0.439666936152464</v>
       </c>
       <c r="K23" t="n">
-        <v>0</v>
+        <v>0.103592130638498</v>
       </c>
       <c r="L23" t="n">
-        <v>0.600803757766292</v>
+        <v>0.35092581817</v>
       </c>
       <c r="M23" t="n">
         <v>0</v>
       </c>
       <c r="N23" t="n">
-        <v>0</v>
+        <v>0.145516824319897</v>
       </c>
       <c r="O23" t="n">
-        <v>0</v>
+        <v>0.527877184889215</v>
       </c>
       <c r="P23" t="n">
-        <v>0</v>
+        <v>0.331272330133863</v>
       </c>
       <c r="Q23" t="n">
-        <v>0</v>
+        <v>0.306394465658784</v>
       </c>
       <c r="R23" t="n">
-        <v>0</v>
+        <v>7.40888549351395</v>
       </c>
       <c r="S23" t="n">
-        <v>0</v>
+        <v>7.89621844327665</v>
       </c>
       <c r="T23" t="n">
-        <v>0</v>
+        <v>15.9112971808729</v>
       </c>
       <c r="U23" t="n">
-        <v>0.0980207775058803</v>
+        <v>1.21014280191541</v>
       </c>
       <c r="V23" t="n">
-        <v>0.146757767840608</v>
+        <v>8.28824020156893</v>
       </c>
     </row>
     <row r="24">
@@ -2224,67 +2251,67 @@
         <v>44</v>
       </c>
       <c r="B24" t="n">
-        <v>0.841079369137107</v>
+        <v>0.933430625359481</v>
       </c>
       <c r="C24" t="n">
-        <v>0.299155633179274</v>
+        <v>0.0134591091250558</v>
       </c>
       <c r="D24" t="n">
-        <v>2.07367676782105</v>
+        <v>0</v>
       </c>
       <c r="E24" t="n">
-        <v>0.412203514162996</v>
+        <v>0</v>
       </c>
       <c r="F24" t="n">
-        <v>0.0489769264257727</v>
+        <v>0</v>
       </c>
       <c r="G24" t="n">
-        <v>0.496597688985074</v>
+        <v>0</v>
       </c>
       <c r="H24" t="n">
-        <v>0.0695525508347812</v>
+        <v>0</v>
       </c>
       <c r="I24" t="n">
-        <v>0.410920131741457</v>
+        <v>0</v>
       </c>
       <c r="J24" t="n">
-        <v>4.8768430070403</v>
+        <v>0</v>
       </c>
       <c r="K24" t="n">
-        <v>0.0424644248646201</v>
+        <v>0</v>
       </c>
       <c r="L24" t="n">
-        <v>5.27289759520598</v>
+        <v>1.03661799078214</v>
       </c>
       <c r="M24" t="n">
-        <v>0.592022452285881</v>
+        <v>0</v>
       </c>
       <c r="N24" t="n">
-        <v>0.235422402117646</v>
+        <v>0</v>
       </c>
       <c r="O24" t="n">
-        <v>4.44346547443995</v>
+        <v>0</v>
       </c>
       <c r="P24" t="n">
-        <v>0.911291683251566</v>
+        <v>0</v>
       </c>
       <c r="Q24" t="n">
-        <v>8.672311178311</v>
+        <v>0</v>
       </c>
       <c r="R24" t="n">
-        <v>4.8333258974333</v>
+        <v>0</v>
       </c>
       <c r="S24" t="n">
-        <v>6.63791461456831</v>
+        <v>0</v>
       </c>
       <c r="T24" t="n">
-        <v>2.95595475726147</v>
+        <v>0</v>
       </c>
       <c r="U24" t="n">
-        <v>3.45312160845392</v>
+        <v>0.0714898929832278</v>
       </c>
       <c r="V24" t="n">
-        <v>5.04697002750521</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
@@ -2292,10 +2319,10 @@
         <v>45</v>
       </c>
       <c r="B25" t="n">
-        <v>0.814213978411628</v>
+        <v>0.825796479935354</v>
       </c>
       <c r="C25" t="n">
-        <v>0.140721659745164</v>
+        <v>0.0854778514098342</v>
       </c>
       <c r="D25" t="n">
         <v>0</v>
@@ -2322,7 +2349,7 @@
         <v>0</v>
       </c>
       <c r="L25" t="n">
-        <v>1.07878699112447</v>
+        <v>0.766307810834754</v>
       </c>
       <c r="M25" t="n">
         <v>0</v>
@@ -2331,7 +2358,7 @@
         <v>0</v>
       </c>
       <c r="O25" t="n">
-        <v>0</v>
+        <v>0.00699522013834512</v>
       </c>
       <c r="P25" t="n">
         <v>0</v>
@@ -2349,10 +2376,10 @@
         <v>0</v>
       </c>
       <c r="U25" t="n">
-        <v>0</v>
+        <v>0.13838730900647</v>
       </c>
       <c r="V25" t="n">
-        <v>0.0491054731373788</v>
+        <v>0.200145959150051</v>
       </c>
     </row>
     <row r="26">
@@ -2360,10 +2387,10 @@
         <v>46</v>
       </c>
       <c r="B26" t="n">
-        <v>0.736312155014346</v>
+        <v>0.785749646850942</v>
       </c>
       <c r="C26" t="n">
-        <v>0.0232232208616773</v>
+        <v>0.0439697587327103</v>
       </c>
       <c r="D26" t="n">
         <v>0</v>
@@ -2390,7 +2417,7 @@
         <v>0</v>
       </c>
       <c r="L26" t="n">
-        <v>0.536936540596519</v>
+        <v>0.44550056840737</v>
       </c>
       <c r="M26" t="n">
         <v>0</v>
@@ -2417,10 +2444,10 @@
         <v>0</v>
       </c>
       <c r="U26" t="n">
-        <v>0.0517281552272252</v>
+        <v>0.0543660839245519</v>
       </c>
       <c r="V26" t="n">
-        <v>0.160612326814521</v>
+        <v>0.0525757146829842</v>
       </c>
     </row>
     <row r="27">
@@ -2428,67 +2455,67 @@
         <v>47</v>
       </c>
       <c r="B27" t="n">
-        <v>0.37528243478537</v>
+        <v>0.658627197823507</v>
       </c>
       <c r="C27" t="n">
-        <v>0.447765815566341</v>
+        <v>0.162419925805785</v>
       </c>
       <c r="D27" t="n">
-        <v>0</v>
+        <v>0.175675414033704</v>
       </c>
       <c r="E27" t="n">
-        <v>0</v>
+        <v>0.185986012955751</v>
       </c>
       <c r="F27" t="n">
-        <v>5.9000190465825</v>
+        <v>0.00147011906433047</v>
       </c>
       <c r="G27" t="n">
-        <v>0</v>
+        <v>0.0334281949665203</v>
       </c>
       <c r="H27" t="n">
-        <v>0.549157219223415</v>
+        <v>0.0207824315444907</v>
       </c>
       <c r="I27" t="n">
-        <v>0</v>
+        <v>0.015971256937921</v>
       </c>
       <c r="J27" t="n">
-        <v>3.90839876585356</v>
+        <v>0.623799543762262</v>
       </c>
       <c r="K27" t="n">
-        <v>0</v>
+        <v>0.0237427802795707</v>
       </c>
       <c r="L27" t="n">
-        <v>0.482298217979411</v>
+        <v>3.90989378054439</v>
       </c>
       <c r="M27" t="n">
-        <v>18.9760360392915</v>
+        <v>0.00986730532122797</v>
       </c>
       <c r="N27" t="n">
-        <v>0</v>
+        <v>0.0977981901932705</v>
       </c>
       <c r="O27" t="n">
-        <v>3.09298296790632</v>
+        <v>0.460020467952493</v>
       </c>
       <c r="P27" t="n">
-        <v>0</v>
+        <v>0.0978345205543062</v>
       </c>
       <c r="Q27" t="n">
-        <v>2.00140728858211</v>
+        <v>0.844954178046066</v>
       </c>
       <c r="R27" t="n">
-        <v>0</v>
+        <v>1.76619842899229</v>
       </c>
       <c r="S27" t="n">
-        <v>0</v>
+        <v>1.41493122396836</v>
       </c>
       <c r="T27" t="n">
-        <v>0</v>
+        <v>2.16546360352325</v>
       </c>
       <c r="U27" t="n">
-        <v>0.250179463179519</v>
+        <v>1.91523372843709</v>
       </c>
       <c r="V27" t="n">
-        <v>0</v>
+        <v>1.80806822074235</v>
       </c>
     </row>
     <row r="28">
@@ -2496,10 +2523,10 @@
         <v>48</v>
       </c>
       <c r="B28" t="n">
-        <v>0.587745503008234</v>
+        <v>0.637589614854246</v>
       </c>
       <c r="C28" t="n">
-        <v>0.0975928210020488</v>
+        <v>0.0764017086764322</v>
       </c>
       <c r="D28" t="n">
         <v>0</v>
@@ -2514,7 +2541,7 @@
         <v>0</v>
       </c>
       <c r="H28" t="n">
-        <v>0.0466919193525119</v>
+        <v>0</v>
       </c>
       <c r="I28" t="n">
         <v>0</v>
@@ -2523,16 +2550,16 @@
         <v>0</v>
       </c>
       <c r="K28" t="n">
-        <v>0.0823888546446672</v>
+        <v>0</v>
       </c>
       <c r="L28" t="n">
-        <v>0.435609267661355</v>
+        <v>0.799928781276662</v>
       </c>
       <c r="M28" t="n">
         <v>0</v>
       </c>
       <c r="N28" t="n">
-        <v>0.0532686531796473</v>
+        <v>0</v>
       </c>
       <c r="O28" t="n">
         <v>0</v>
@@ -2556,7 +2583,7 @@
         <v>0</v>
       </c>
       <c r="V28" t="n">
-        <v>0</v>
+        <v>0.0175919502117789</v>
       </c>
     </row>
     <row r="29">
@@ -2564,67 +2591,67 @@
         <v>49</v>
       </c>
       <c r="B29" t="n">
-        <v>0.454238568574496</v>
+        <v>0.270644835553678</v>
       </c>
       <c r="C29" t="n">
-        <v>0.136261326849508</v>
+        <v>0.42888026616414</v>
       </c>
       <c r="D29" t="n">
-        <v>1.95976202889649</v>
+        <v>0.337091885673534</v>
       </c>
       <c r="E29" t="n">
-        <v>0</v>
+        <v>1.66321808981638</v>
       </c>
       <c r="F29" t="n">
-        <v>0</v>
+        <v>3.64859049782417</v>
       </c>
       <c r="G29" t="n">
-        <v>0</v>
+        <v>3.10791163630364</v>
       </c>
       <c r="H29" t="n">
-        <v>0</v>
+        <v>0.749707715802749</v>
       </c>
       <c r="I29" t="n">
-        <v>0</v>
+        <v>4.88947480166689</v>
       </c>
       <c r="J29" t="n">
-        <v>0</v>
+        <v>4.19444172670021</v>
       </c>
       <c r="K29" t="n">
-        <v>0</v>
+        <v>1.45608050702737</v>
       </c>
       <c r="L29" t="n">
-        <v>1.12162376274282</v>
+        <v>0.197769226910463</v>
       </c>
       <c r="M29" t="n">
-        <v>0</v>
+        <v>18.0883265361352</v>
       </c>
       <c r="N29" t="n">
-        <v>0</v>
+        <v>2.99812076615919</v>
       </c>
       <c r="O29" t="n">
-        <v>0</v>
+        <v>7.84881161892712</v>
       </c>
       <c r="P29" t="n">
-        <v>0</v>
+        <v>1.22413242166558</v>
       </c>
       <c r="Q29" t="n">
-        <v>0</v>
+        <v>4.64782438811394</v>
       </c>
       <c r="R29" t="n">
-        <v>0.12607271981775</v>
+        <v>0.00108022533500488</v>
       </c>
       <c r="S29" t="n">
-        <v>0.115924595999734</v>
+        <v>0</v>
       </c>
       <c r="T29" t="n">
-        <v>0</v>
+        <v>0.25611955449373</v>
       </c>
       <c r="U29" t="n">
-        <v>0.672158004420175</v>
+        <v>0</v>
       </c>
       <c r="V29" t="n">
-        <v>0.902725074433339</v>
+        <v>0.0420485635892462</v>
       </c>
     </row>
     <row r="30">
@@ -2632,10 +2659,10 @@
         <v>50</v>
       </c>
       <c r="B30" t="n">
-        <v>0.519840104066944</v>
+        <v>0.576586739819833</v>
       </c>
       <c r="C30" t="n">
-        <v>0.0321070243976523</v>
+        <v>0.0126085334554426</v>
       </c>
       <c r="D30" t="n">
         <v>0</v>
@@ -2662,7 +2689,7 @@
         <v>0</v>
       </c>
       <c r="L30" t="n">
-        <v>0.340284859767083</v>
+        <v>0.39814253979331</v>
       </c>
       <c r="M30" t="n">
         <v>0</v>
@@ -2689,10 +2716,10 @@
         <v>0</v>
       </c>
       <c r="U30" t="n">
-        <v>0.0946507470777669</v>
+        <v>0.028690419520258</v>
       </c>
       <c r="V30" t="n">
-        <v>0.0683789523551214</v>
+        <v>0.0575390863013245</v>
       </c>
     </row>
     <row r="31">
@@ -2700,10 +2727,10 @@
         <v>51</v>
       </c>
       <c r="B31" t="n">
-        <v>0.515349522768354</v>
+        <v>0.293873833415571</v>
       </c>
       <c r="C31" t="n">
-        <v>0</v>
+        <v>0.243104533148035</v>
       </c>
       <c r="D31" t="n">
         <v>0</v>
@@ -2712,40 +2739,40 @@
         <v>0</v>
       </c>
       <c r="F31" t="n">
-        <v>0</v>
+        <v>0.177098301450977</v>
       </c>
       <c r="G31" t="n">
         <v>0</v>
       </c>
       <c r="H31" t="n">
-        <v>0</v>
+        <v>0.164089198436217</v>
       </c>
       <c r="I31" t="n">
         <v>0</v>
       </c>
       <c r="J31" t="n">
-        <v>0</v>
+        <v>0.499925333553042</v>
       </c>
       <c r="K31" t="n">
         <v>0</v>
       </c>
       <c r="L31" t="n">
-        <v>0.181882727157397</v>
+        <v>0.357627806874121</v>
       </c>
       <c r="M31" t="n">
-        <v>0</v>
+        <v>0.316275743704223</v>
       </c>
       <c r="N31" t="n">
         <v>0</v>
       </c>
       <c r="O31" t="n">
-        <v>0</v>
+        <v>0.320208513028829</v>
       </c>
       <c r="P31" t="n">
         <v>0</v>
       </c>
       <c r="Q31" t="n">
-        <v>0</v>
+        <v>0.194999627629674</v>
       </c>
       <c r="R31" t="n">
         <v>0</v>
@@ -2757,10 +2784,10 @@
         <v>0</v>
       </c>
       <c r="U31" t="n">
-        <v>0</v>
+        <v>0.138759128804106</v>
       </c>
       <c r="V31" t="n">
-        <v>0.0125696603593973</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32">
@@ -2768,10 +2795,10 @@
         <v>52</v>
       </c>
       <c r="B32" t="n">
-        <v>0.390888831820181</v>
+        <v>0.460248090589626</v>
       </c>
       <c r="C32" t="n">
-        <v>0</v>
+        <v>0.0529858608306101</v>
       </c>
       <c r="D32" t="n">
         <v>0</v>
@@ -2786,7 +2813,7 @@
         <v>0</v>
       </c>
       <c r="H32" t="n">
-        <v>0</v>
+        <v>0.0139516323409839</v>
       </c>
       <c r="I32" t="n">
         <v>0</v>
@@ -2795,16 +2822,16 @@
         <v>0</v>
       </c>
       <c r="K32" t="n">
-        <v>0.0263300898907838</v>
+        <v>0.0460653942576676</v>
       </c>
       <c r="L32" t="n">
-        <v>0.369604976089268</v>
+        <v>0.323007594140484</v>
       </c>
       <c r="M32" t="n">
         <v>0</v>
       </c>
       <c r="N32" t="n">
-        <v>0.072052355476268</v>
+        <v>0.022128641234402</v>
       </c>
       <c r="O32" t="n">
         <v>0</v>
@@ -2816,7 +2843,7 @@
         <v>0</v>
       </c>
       <c r="R32" t="n">
-        <v>0.0160396469416417</v>
+        <v>0</v>
       </c>
       <c r="S32" t="n">
         <v>0</v>
@@ -2836,13 +2863,13 @@
         <v>53</v>
       </c>
       <c r="B33" t="n">
-        <v>0.368982604789667</v>
+        <v>0.355702311269998</v>
       </c>
       <c r="C33" t="n">
-        <v>0</v>
+        <v>0.0739800697111805</v>
       </c>
       <c r="D33" t="n">
-        <v>0</v>
+        <v>0.166024913417766</v>
       </c>
       <c r="E33" t="n">
         <v>0</v>
@@ -2866,7 +2893,7 @@
         <v>0</v>
       </c>
       <c r="L33" t="n">
-        <v>0.154155207682796</v>
+        <v>0.831692574125862</v>
       </c>
       <c r="M33" t="n">
         <v>0</v>
@@ -2884,19 +2911,19 @@
         <v>0</v>
       </c>
       <c r="R33" t="n">
-        <v>0</v>
+        <v>0.0460696101206712</v>
       </c>
       <c r="S33" t="n">
-        <v>0</v>
+        <v>0.0247103706555598</v>
       </c>
       <c r="T33" t="n">
         <v>0</v>
       </c>
       <c r="U33" t="n">
-        <v>0</v>
+        <v>0.372804617640116</v>
       </c>
       <c r="V33" t="n">
-        <v>0</v>
+        <v>0.323399685406296</v>
       </c>
     </row>
     <row r="34">
@@ -2904,10 +2931,10 @@
         <v>54</v>
       </c>
       <c r="B34" t="n">
-        <v>0.304136007602489</v>
+        <v>0.407073153404241</v>
       </c>
       <c r="C34" t="n">
-        <v>0</v>
+        <v>0.0174317978407786</v>
       </c>
       <c r="D34" t="n">
         <v>0</v>
@@ -2934,7 +2961,7 @@
         <v>0</v>
       </c>
       <c r="L34" t="n">
-        <v>0.289212865133454</v>
+        <v>0.252323818696267</v>
       </c>
       <c r="M34" t="n">
         <v>0</v>
@@ -2961,10 +2988,10 @@
         <v>0</v>
       </c>
       <c r="U34" t="n">
-        <v>0</v>
+        <v>0.0524969357526542</v>
       </c>
       <c r="V34" t="n">
-        <v>0.0428485755362566</v>
+        <v>0.0244966405679378</v>
       </c>
     </row>
     <row r="35">
@@ -2972,7 +2999,7 @@
         <v>55</v>
       </c>
       <c r="B35" t="n">
-        <v>0.21972609536667</v>
+        <v>0.403556696948623</v>
       </c>
       <c r="C35" t="n">
         <v>0</v>
@@ -3002,7 +3029,7 @@
         <v>0</v>
       </c>
       <c r="L35" t="n">
-        <v>0.293133103527507</v>
+        <v>0.134867429313954</v>
       </c>
       <c r="M35" t="n">
         <v>0</v>
@@ -3032,7 +3059,7 @@
         <v>0</v>
       </c>
       <c r="V35" t="n">
-        <v>0</v>
+        <v>0.00450305892792974</v>
       </c>
     </row>
     <row r="36">
@@ -3040,10 +3067,10 @@
         <v>56</v>
       </c>
       <c r="B36" t="n">
-        <v>0.15791226757825</v>
+        <v>0.306094793677269</v>
       </c>
       <c r="C36" t="n">
-        <v>0.0711441527984718</v>
+        <v>0</v>
       </c>
       <c r="D36" t="n">
         <v>0</v>
@@ -3064,22 +3091,22 @@
         <v>0</v>
       </c>
       <c r="J36" t="n">
-        <v>0.762243235061095</v>
+        <v>0</v>
       </c>
       <c r="K36" t="n">
-        <v>0</v>
+        <v>0.0147217239138703</v>
       </c>
       <c r="L36" t="n">
-        <v>0.47056472667499</v>
+        <v>0.274064908558732</v>
       </c>
       <c r="M36" t="n">
         <v>0</v>
       </c>
       <c r="N36" t="n">
-        <v>0</v>
+        <v>0.0299316883242906</v>
       </c>
       <c r="O36" t="n">
-        <v>0.538863455512759</v>
+        <v>0</v>
       </c>
       <c r="P36" t="n">
         <v>0</v>
@@ -3088,7 +3115,7 @@
         <v>0</v>
       </c>
       <c r="R36" t="n">
-        <v>0</v>
+        <v>0.00586122265104501</v>
       </c>
       <c r="S36" t="n">
         <v>0</v>
@@ -3097,7 +3124,7 @@
         <v>0</v>
       </c>
       <c r="U36" t="n">
-        <v>0.175459003579842</v>
+        <v>0</v>
       </c>
       <c r="V36" t="n">
         <v>0</v>
@@ -3108,10 +3135,10 @@
         <v>57</v>
       </c>
       <c r="B37" t="n">
-        <v>0.138440065773349</v>
+        <v>0.288940601750298</v>
       </c>
       <c r="C37" t="n">
-        <v>0.0401982894439034</v>
+        <v>0</v>
       </c>
       <c r="D37" t="n">
         <v>0</v>
@@ -3138,13 +3165,13 @@
         <v>0</v>
       </c>
       <c r="L37" t="n">
-        <v>0.0269652508979796</v>
+        <v>0.114307262159896</v>
       </c>
       <c r="M37" t="n">
         <v>0</v>
       </c>
       <c r="N37" t="n">
-        <v>0.0568327402820831</v>
+        <v>0</v>
       </c>
       <c r="O37" t="n">
         <v>0</v>
@@ -3168,7 +3195,7 @@
         <v>0</v>
       </c>
       <c r="V37" t="n">
-        <v>0.043826215786432</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38">
@@ -3176,10 +3203,10 @@
         <v>58</v>
       </c>
       <c r="B38" t="n">
-        <v>0.136513671477142</v>
+        <v>0.103873065910727</v>
       </c>
       <c r="C38" t="n">
-        <v>0</v>
+        <v>0.165492004988977</v>
       </c>
       <c r="D38" t="n">
         <v>0</v>
@@ -3206,7 +3233,7 @@
         <v>0</v>
       </c>
       <c r="L38" t="n">
-        <v>0.0635541425758035</v>
+        <v>0.45315133262081</v>
       </c>
       <c r="M38" t="n">
         <v>0</v>
@@ -3218,25 +3245,25 @@
         <v>0</v>
       </c>
       <c r="P38" t="n">
-        <v>0</v>
+        <v>0.258226691270741</v>
       </c>
       <c r="Q38" t="n">
         <v>0</v>
       </c>
       <c r="R38" t="n">
-        <v>0</v>
+        <v>0.03711774276114</v>
       </c>
       <c r="S38" t="n">
-        <v>0</v>
+        <v>0.0219003285049276</v>
       </c>
       <c r="T38" t="n">
-        <v>0</v>
+        <v>0.191649185085521</v>
       </c>
       <c r="U38" t="n">
-        <v>0</v>
+        <v>0.244185115209369</v>
       </c>
       <c r="V38" t="n">
-        <v>0</v>
+        <v>0.151052610037999</v>
       </c>
     </row>
     <row r="39">
@@ -3244,64 +3271,64 @@
         <v>59</v>
       </c>
       <c r="B39" t="n">
-        <v>0.135133956643372</v>
+        <v>0</v>
       </c>
       <c r="C39" t="n">
-        <v>0</v>
+        <v>0.255172700883958</v>
       </c>
       <c r="D39" t="n">
         <v>0</v>
       </c>
       <c r="E39" t="n">
-        <v>0</v>
+        <v>0.156429665934569</v>
       </c>
       <c r="F39" t="n">
         <v>0</v>
       </c>
       <c r="G39" t="n">
-        <v>0</v>
+        <v>0.188622667317821</v>
       </c>
       <c r="H39" t="n">
         <v>0</v>
       </c>
       <c r="I39" t="n">
-        <v>0</v>
+        <v>0.198095590122943</v>
       </c>
       <c r="J39" t="n">
-        <v>1.16917017178855</v>
+        <v>0.388244926543664</v>
       </c>
       <c r="K39" t="n">
         <v>0</v>
       </c>
       <c r="L39" t="n">
-        <v>0.19978242676913</v>
+        <v>0</v>
       </c>
       <c r="M39" t="n">
-        <v>0</v>
+        <v>0.0885447611785879</v>
       </c>
       <c r="N39" t="n">
-        <v>0</v>
+        <v>0.0050319649823256</v>
       </c>
       <c r="O39" t="n">
-        <v>0.365030133093618</v>
+        <v>0.37294487160484</v>
       </c>
       <c r="P39" t="n">
-        <v>0.105987995484557</v>
+        <v>0.578360537221201</v>
       </c>
       <c r="Q39" t="n">
-        <v>0.58364780927889</v>
+        <v>0.371839825669476</v>
       </c>
       <c r="R39" t="n">
-        <v>0.126319062518219</v>
+        <v>0.00349072816589541</v>
       </c>
       <c r="S39" t="n">
         <v>0</v>
       </c>
       <c r="T39" t="n">
-        <v>0</v>
+        <v>0.0202020505381624</v>
       </c>
       <c r="U39" t="n">
-        <v>0.0573629910505762</v>
+        <v>0</v>
       </c>
       <c r="V39" t="n">
         <v>0</v>
@@ -3312,7 +3339,7 @@
         <v>60</v>
       </c>
       <c r="B40" t="n">
-        <v>0.123237170246528</v>
+        <v>0.238160932005696</v>
       </c>
       <c r="C40" t="n">
         <v>0</v>
@@ -3342,13 +3369,13 @@
         <v>0</v>
       </c>
       <c r="L40" t="n">
-        <v>0</v>
+        <v>0.214453545175391</v>
       </c>
       <c r="M40" t="n">
         <v>0</v>
       </c>
       <c r="N40" t="n">
-        <v>0.0183983955828438</v>
+        <v>0</v>
       </c>
       <c r="O40" t="n">
         <v>0</v>
@@ -3372,7 +3399,7 @@
         <v>0</v>
       </c>
       <c r="V40" t="n">
-        <v>0</v>
+        <v>0.0153504275454316</v>
       </c>
     </row>
     <row r="41">
@@ -3380,7 +3407,7 @@
         <v>61</v>
       </c>
       <c r="B41" t="n">
-        <v>0.119228187521989</v>
+        <v>0.172061743267489</v>
       </c>
       <c r="C41" t="n">
         <v>0</v>
@@ -3395,25 +3422,25 @@
         <v>0</v>
       </c>
       <c r="G41" t="n">
-        <v>0.691907285910062</v>
+        <v>0</v>
       </c>
       <c r="H41" t="n">
-        <v>0.0433113574495702</v>
+        <v>0</v>
       </c>
       <c r="I41" t="n">
         <v>0</v>
       </c>
       <c r="J41" t="n">
-        <v>0.675688732294572</v>
+        <v>0</v>
       </c>
       <c r="K41" t="n">
         <v>0</v>
       </c>
       <c r="L41" t="n">
-        <v>0.0629007695101281</v>
+        <v>0.217360431842238</v>
       </c>
       <c r="M41" t="n">
-        <v>0.664293758770424</v>
+        <v>0</v>
       </c>
       <c r="N41" t="n">
         <v>0</v>
@@ -3448,10 +3475,10 @@
         <v>62</v>
       </c>
       <c r="B42" t="n">
-        <v>0.10334845075596</v>
+        <v>0.123656955708855</v>
       </c>
       <c r="C42" t="n">
-        <v>0</v>
+        <v>0.0386261421730227</v>
       </c>
       <c r="D42" t="n">
         <v>0</v>
@@ -3472,13 +3499,13 @@
         <v>0</v>
       </c>
       <c r="J42" t="n">
-        <v>0</v>
+        <v>0.097498931497397</v>
       </c>
       <c r="K42" t="n">
         <v>0</v>
       </c>
       <c r="L42" t="n">
-        <v>0.0322739070565925</v>
+        <v>0.348927333586542</v>
       </c>
       <c r="M42" t="n">
         <v>0</v>
@@ -3487,7 +3514,7 @@
         <v>0</v>
       </c>
       <c r="O42" t="n">
-        <v>0</v>
+        <v>0.0557871374028669</v>
       </c>
       <c r="P42" t="n">
         <v>0</v>
@@ -3505,7 +3532,7 @@
         <v>0</v>
       </c>
       <c r="U42" t="n">
-        <v>0</v>
+        <v>0.09731629514332</v>
       </c>
       <c r="V42" t="n">
         <v>0</v>
@@ -3516,10 +3543,10 @@
         <v>63</v>
       </c>
       <c r="B43" t="n">
-        <v>0.0584686701254122</v>
+        <v>0.108408785107104</v>
       </c>
       <c r="C43" t="n">
-        <v>0.0425206115300711</v>
+        <v>0.0218247710050162</v>
       </c>
       <c r="D43" t="n">
         <v>0</v>
@@ -3534,7 +3561,7 @@
         <v>0</v>
       </c>
       <c r="H43" t="n">
-        <v>0.00692847835553403</v>
+        <v>0</v>
       </c>
       <c r="I43" t="n">
         <v>0</v>
@@ -3543,16 +3570,16 @@
         <v>0</v>
       </c>
       <c r="K43" t="n">
-        <v>0.0197475674180878</v>
+        <v>0</v>
       </c>
       <c r="L43" t="n">
-        <v>0.14547079068486</v>
+        <v>0.0199949391910599</v>
       </c>
       <c r="M43" t="n">
         <v>0</v>
       </c>
       <c r="N43" t="n">
-        <v>0</v>
+        <v>0.0236092194001758</v>
       </c>
       <c r="O43" t="n">
         <v>0</v>
@@ -3576,7 +3603,7 @@
         <v>0</v>
       </c>
       <c r="V43" t="n">
-        <v>0</v>
+        <v>0.0157006654620484</v>
       </c>
     </row>
     <row r="44">
@@ -3584,7 +3611,7 @@
         <v>64</v>
       </c>
       <c r="B44" t="n">
-        <v>0.08444896076885</v>
+        <v>0.106900276250781</v>
       </c>
       <c r="C44" t="n">
         <v>0</v>
@@ -3614,7 +3641,7 @@
         <v>0</v>
       </c>
       <c r="L44" t="n">
-        <v>0.0674879929087243</v>
+        <v>0.0471258814149715</v>
       </c>
       <c r="M44" t="n">
         <v>0</v>
@@ -3632,7 +3659,7 @@
         <v>0</v>
       </c>
       <c r="R44" t="n">
-        <v>0.068729613430823</v>
+        <v>0</v>
       </c>
       <c r="S44" t="n">
         <v>0</v>
@@ -3641,10 +3668,10 @@
         <v>0</v>
       </c>
       <c r="U44" t="n">
-        <v>0.143008871876879</v>
+        <v>0</v>
       </c>
       <c r="V44" t="n">
-        <v>0.0651108406616781</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45">
@@ -3652,7 +3679,7 @@
         <v>65</v>
       </c>
       <c r="B45" t="n">
-        <v>0.08284797091457</v>
+        <v>0.105819857745576</v>
       </c>
       <c r="C45" t="n">
         <v>0</v>
@@ -3676,13 +3703,13 @@
         <v>0</v>
       </c>
       <c r="J45" t="n">
-        <v>0</v>
+        <v>0.149549169142675</v>
       </c>
       <c r="K45" t="n">
         <v>0</v>
       </c>
       <c r="L45" t="n">
-        <v>0</v>
+        <v>0.148140193087928</v>
       </c>
       <c r="M45" t="n">
         <v>0</v>
@@ -3691,16 +3718,16 @@
         <v>0</v>
       </c>
       <c r="O45" t="n">
-        <v>0</v>
+        <v>0.0377906239191948</v>
       </c>
       <c r="P45" t="n">
-        <v>0</v>
+        <v>0.0113786671307535</v>
       </c>
       <c r="Q45" t="n">
-        <v>0</v>
+        <v>0.0568655396258137</v>
       </c>
       <c r="R45" t="n">
-        <v>0</v>
+        <v>0.0461596288985882</v>
       </c>
       <c r="S45" t="n">
         <v>0</v>
@@ -3709,7 +3736,7 @@
         <v>0</v>
       </c>
       <c r="U45" t="n">
-        <v>0</v>
+        <v>0.0318157156571407</v>
       </c>
       <c r="V45" t="n">
         <v>0</v>
@@ -3720,7 +3747,7 @@
         <v>66</v>
       </c>
       <c r="B46" t="n">
-        <v>0.0770818042036266</v>
+        <v>0.0965037962950411</v>
       </c>
       <c r="C46" t="n">
         <v>0</v>
@@ -3750,13 +3777,13 @@
         <v>0</v>
       </c>
       <c r="L46" t="n">
-        <v>0.0042197010491538</v>
+        <v>0</v>
       </c>
       <c r="M46" t="n">
         <v>0</v>
       </c>
       <c r="N46" t="n">
-        <v>0</v>
+        <v>0.00764298458548063</v>
       </c>
       <c r="O46" t="n">
         <v>0</v>
@@ -3788,40 +3815,40 @@
         <v>67</v>
       </c>
       <c r="B47" t="n">
-        <v>0</v>
+        <v>0.0933644670535041</v>
       </c>
       <c r="C47" t="n">
-        <v>0.0971689050656849</v>
+        <v>0</v>
       </c>
       <c r="D47" t="n">
         <v>0</v>
       </c>
       <c r="E47" t="n">
-        <v>0.958058387483828</v>
+        <v>0</v>
       </c>
       <c r="F47" t="n">
         <v>0</v>
       </c>
       <c r="G47" t="n">
-        <v>0</v>
+        <v>0.0465753509635294</v>
       </c>
       <c r="H47" t="n">
-        <v>0</v>
+        <v>0.0129415141571564</v>
       </c>
       <c r="I47" t="n">
         <v>0</v>
       </c>
       <c r="J47" t="n">
-        <v>0</v>
+        <v>0.0864276997069986</v>
       </c>
       <c r="K47" t="n">
         <v>0</v>
       </c>
       <c r="L47" t="n">
-        <v>0</v>
+        <v>0.0466414003038302</v>
       </c>
       <c r="M47" t="n">
-        <v>0</v>
+        <v>0.0110718593787533</v>
       </c>
       <c r="N47" t="n">
         <v>0</v>
@@ -3839,16 +3866,16 @@
         <v>0</v>
       </c>
       <c r="S47" t="n">
-        <v>0.186483314082938</v>
+        <v>0</v>
       </c>
       <c r="T47" t="n">
-        <v>0.214409551761049</v>
+        <v>0</v>
       </c>
       <c r="U47" t="n">
         <v>0</v>
       </c>
       <c r="V47" t="n">
-        <v>0.119272110521392</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48">
@@ -3856,7 +3883,7 @@
         <v>68</v>
       </c>
       <c r="B48" t="n">
-        <v>0.0639094323944287</v>
+        <v>0.0818162202007071</v>
       </c>
       <c r="C48" t="n">
         <v>0</v>
@@ -3886,7 +3913,7 @@
         <v>0</v>
       </c>
       <c r="L48" t="n">
-        <v>0</v>
+        <v>0.0559474749803356</v>
       </c>
       <c r="M48" t="n">
         <v>0</v>
@@ -3924,7 +3951,7 @@
         <v>69</v>
       </c>
       <c r="B49" t="n">
-        <v>0.0567375184943615</v>
+        <v>0.080929461616247</v>
       </c>
       <c r="C49" t="n">
         <v>0</v>
@@ -3954,7 +3981,7 @@
         <v>0</v>
       </c>
       <c r="L49" t="n">
-        <v>0.00578507401900118</v>
+        <v>0.0239313482190828</v>
       </c>
       <c r="M49" t="n">
         <v>0</v>
@@ -3992,10 +4019,10 @@
         <v>70</v>
       </c>
       <c r="B50" t="n">
-        <v>0.0554359007266541</v>
+        <v>0.0457852823148843</v>
       </c>
       <c r="C50" t="n">
-        <v>0</v>
+        <v>0.0230856243505605</v>
       </c>
       <c r="D50" t="n">
         <v>0</v>
@@ -4010,7 +4037,7 @@
         <v>0</v>
       </c>
       <c r="H50" t="n">
-        <v>0</v>
+        <v>0.00207024221833955</v>
       </c>
       <c r="I50" t="n">
         <v>0</v>
@@ -4019,10 +4046,10 @@
         <v>0</v>
       </c>
       <c r="K50" t="n">
-        <v>0</v>
+        <v>0.0110412929354027</v>
       </c>
       <c r="L50" t="n">
-        <v>0.223998066015726</v>
+        <v>0.107867700724309</v>
       </c>
       <c r="M50" t="n">
         <v>0</v>
@@ -4060,7 +4087,7 @@
         <v>71</v>
       </c>
       <c r="B51" t="n">
-        <v>0.0524031313278961</v>
+        <v>0.0661297666204295</v>
       </c>
       <c r="C51" t="n">
         <v>0</v>
@@ -4078,25 +4105,25 @@
         <v>0</v>
       </c>
       <c r="H51" t="n">
-        <v>0.228037309353881</v>
+        <v>0</v>
       </c>
       <c r="I51" t="n">
         <v>0</v>
       </c>
       <c r="J51" t="n">
-        <v>0.169324762156278</v>
+        <v>0</v>
       </c>
       <c r="K51" t="n">
-        <v>0.12243849545001</v>
+        <v>0</v>
       </c>
       <c r="L51" t="n">
-        <v>0</v>
+        <v>0.0500428614383013</v>
       </c>
       <c r="M51" t="n">
         <v>0</v>
       </c>
       <c r="N51" t="n">
-        <v>0.029114738559762</v>
+        <v>0</v>
       </c>
       <c r="O51" t="n">
         <v>0</v>
@@ -4108,7 +4135,7 @@
         <v>0</v>
       </c>
       <c r="R51" t="n">
-        <v>0</v>
+        <v>0.0251152390388635</v>
       </c>
       <c r="S51" t="n">
         <v>0</v>
@@ -4117,10 +4144,10 @@
         <v>0</v>
       </c>
       <c r="U51" t="n">
-        <v>0</v>
+        <v>0.0793182071010145</v>
       </c>
       <c r="V51" t="n">
-        <v>0</v>
+        <v>0.0233258452466761</v>
       </c>
     </row>
     <row r="52">
@@ -4128,10 +4155,10 @@
         <v>72</v>
       </c>
       <c r="B52" t="n">
-        <v>0.0117796407977511</v>
+        <v>0.0648760734492962</v>
       </c>
       <c r="C52" t="n">
-        <v>0.0566019930684215</v>
+        <v>0</v>
       </c>
       <c r="D52" t="n">
         <v>0</v>
@@ -4158,10 +4185,10 @@
         <v>0</v>
       </c>
       <c r="L52" t="n">
-        <v>0.0695978434333012</v>
+        <v>0</v>
       </c>
       <c r="M52" t="n">
-        <v>3.56177088791323</v>
+        <v>0</v>
       </c>
       <c r="N52" t="n">
         <v>0</v>
@@ -4196,7 +4223,7 @@
         <v>73</v>
       </c>
       <c r="B53" t="n">
-        <v>0.0495916369496483</v>
+        <v>0.0603607395077348</v>
       </c>
       <c r="C53" t="n">
         <v>0</v>
@@ -4226,7 +4253,7 @@
         <v>0</v>
       </c>
       <c r="L53" t="n">
-        <v>0.0172191026683212</v>
+        <v>0.00312894050945409</v>
       </c>
       <c r="M53" t="n">
         <v>0</v>
@@ -4264,16 +4291,16 @@
         <v>74</v>
       </c>
       <c r="B54" t="n">
-        <v>0.0428752892682786</v>
+        <v>0</v>
       </c>
       <c r="C54" t="n">
-        <v>0</v>
+        <v>0.0527557050611854</v>
       </c>
       <c r="D54" t="n">
         <v>0</v>
       </c>
       <c r="E54" t="n">
-        <v>0</v>
+        <v>0.432275450219654</v>
       </c>
       <c r="F54" t="n">
         <v>0</v>
@@ -4294,7 +4321,7 @@
         <v>0</v>
       </c>
       <c r="L54" t="n">
-        <v>0.0316885936852582</v>
+        <v>0</v>
       </c>
       <c r="M54" t="n">
         <v>0</v>
@@ -4315,16 +4342,16 @@
         <v>0</v>
       </c>
       <c r="S54" t="n">
-        <v>0</v>
+        <v>0.0397505962589439</v>
       </c>
       <c r="T54" t="n">
-        <v>0</v>
+        <v>0.157071443480559</v>
       </c>
       <c r="U54" t="n">
         <v>0</v>
       </c>
       <c r="V54" t="n">
-        <v>0</v>
+        <v>0.0427290258272445</v>
       </c>
     </row>
     <row r="55">
@@ -4332,13 +4359,13 @@
         <v>75</v>
       </c>
       <c r="B55" t="n">
-        <v>0.0410660405711655</v>
+        <v>0.050045800571256</v>
       </c>
       <c r="C55" t="n">
         <v>0</v>
       </c>
       <c r="D55" t="n">
-        <v>0.279727937798029</v>
+        <v>0</v>
       </c>
       <c r="E55" t="n">
         <v>0</v>
@@ -4362,13 +4389,13 @@
         <v>0</v>
       </c>
       <c r="L55" t="n">
-        <v>0.0108759391557222</v>
+        <v>0</v>
       </c>
       <c r="M55" t="n">
         <v>0</v>
       </c>
       <c r="N55" t="n">
-        <v>0.0159661469521276</v>
+        <v>0</v>
       </c>
       <c r="O55" t="n">
         <v>0</v>
@@ -4400,7 +4427,7 @@
         <v>76</v>
       </c>
       <c r="B56" t="n">
-        <v>0.0406495228854992</v>
+        <v>0.0444296628696751</v>
       </c>
       <c r="C56" t="n">
         <v>0</v>
@@ -4427,25 +4454,25 @@
         <v>0</v>
       </c>
       <c r="K56" t="n">
-        <v>0.0347728904535895</v>
+        <v>0</v>
       </c>
       <c r="L56" t="n">
-        <v>0</v>
+        <v>0.00428967650489674</v>
       </c>
       <c r="M56" t="n">
-        <v>2.75835486416006</v>
+        <v>0</v>
       </c>
       <c r="N56" t="n">
         <v>0</v>
       </c>
       <c r="O56" t="n">
-        <v>1.79786518392399</v>
+        <v>0</v>
       </c>
       <c r="P56" t="n">
         <v>0</v>
       </c>
       <c r="Q56" t="n">
-        <v>2.89363243800182</v>
+        <v>0</v>
       </c>
       <c r="R56" t="n">
         <v>0</v>
@@ -4468,7 +4495,7 @@
         <v>77</v>
       </c>
       <c r="B57" t="n">
-        <v>0.0401939566668016</v>
+        <v>0.0434104001289164</v>
       </c>
       <c r="C57" t="n">
         <v>0</v>
@@ -4498,7 +4525,7 @@
         <v>0</v>
       </c>
       <c r="L57" t="n">
-        <v>0.0151228640826125</v>
+        <v>0.166096274269602</v>
       </c>
       <c r="M57" t="n">
         <v>0</v>
@@ -4536,7 +4563,7 @@
         <v>78</v>
       </c>
       <c r="B58" t="n">
-        <v>0.0345058870219207</v>
+        <v>0.0410355179429484</v>
       </c>
       <c r="C58" t="n">
         <v>0</v>
@@ -4554,25 +4581,25 @@
         <v>0</v>
       </c>
       <c r="H58" t="n">
-        <v>0</v>
+        <v>0.0681379721427407</v>
       </c>
       <c r="I58" t="n">
         <v>0</v>
       </c>
       <c r="J58" t="n">
-        <v>0</v>
+        <v>0.0216584190281003</v>
       </c>
       <c r="K58" t="n">
-        <v>0</v>
+        <v>0.0684580164337244</v>
       </c>
       <c r="L58" t="n">
-        <v>0.0455455474531246</v>
+        <v>0</v>
       </c>
       <c r="M58" t="n">
         <v>0</v>
       </c>
       <c r="N58" t="n">
-        <v>0</v>
+        <v>0.0120947229893273</v>
       </c>
       <c r="O58" t="n">
         <v>0</v>
@@ -4604,10 +4631,10 @@
         <v>79</v>
       </c>
       <c r="B59" t="n">
-        <v>0.0165435618275599</v>
+        <v>0.00922432780386694</v>
       </c>
       <c r="C59" t="n">
-        <v>0.00914183932332695</v>
+        <v>0.0307307986044955</v>
       </c>
       <c r="D59" t="n">
         <v>0</v>
@@ -4616,13 +4643,13 @@
         <v>0</v>
       </c>
       <c r="F59" t="n">
-        <v>0.279576621680453</v>
+        <v>0</v>
       </c>
       <c r="G59" t="n">
         <v>0</v>
       </c>
       <c r="H59" t="n">
-        <v>0.142418721752644</v>
+        <v>0</v>
       </c>
       <c r="I59" t="n">
         <v>0</v>
@@ -4634,25 +4661,25 @@
         <v>0</v>
       </c>
       <c r="L59" t="n">
-        <v>0.0259443554828618</v>
+        <v>0.0516073316930283</v>
       </c>
       <c r="M59" t="n">
-        <v>0</v>
+        <v>0.0593644391350378</v>
       </c>
       <c r="N59" t="n">
         <v>0</v>
       </c>
       <c r="O59" t="n">
-        <v>0.61565968356779</v>
+        <v>0</v>
       </c>
       <c r="P59" t="n">
-        <v>0.0594725955313522</v>
+        <v>0</v>
       </c>
       <c r="Q59" t="n">
-        <v>0.101358284783273</v>
+        <v>0</v>
       </c>
       <c r="R59" t="n">
-        <v>0.00925153697316534</v>
+        <v>0</v>
       </c>
       <c r="S59" t="n">
         <v>0</v>
@@ -4664,7 +4691,7 @@
         <v>0</v>
       </c>
       <c r="V59" t="n">
-        <v>0.0164802213600987</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60">
@@ -4672,7 +4699,7 @@
         <v>80</v>
       </c>
       <c r="B60" t="n">
-        <v>0.0156454455678418</v>
+        <v>0.0388339104229094</v>
       </c>
       <c r="C60" t="n">
         <v>0</v>
@@ -4702,7 +4729,7 @@
         <v>0</v>
       </c>
       <c r="L60" t="n">
-        <v>0.0474784427724144</v>
+        <v>0.0127680959498691</v>
       </c>
       <c r="M60" t="n">
         <v>0</v>
@@ -4740,7 +4767,7 @@
         <v>81</v>
       </c>
       <c r="B61" t="n">
-        <v>0.0145520866429677</v>
+        <v>0.0335745146805941</v>
       </c>
       <c r="C61" t="n">
         <v>0</v>
@@ -4770,7 +4797,7 @@
         <v>0</v>
       </c>
       <c r="L61" t="n">
-        <v>0.0121690733482048</v>
+        <v>0.023497333890352</v>
       </c>
       <c r="M61" t="n">
         <v>0</v>
@@ -4808,13 +4835,13 @@
         <v>82</v>
       </c>
       <c r="B62" t="n">
-        <v>0.0115583657772409</v>
+        <v>0.0321577394709394</v>
       </c>
       <c r="C62" t="n">
         <v>0</v>
       </c>
       <c r="D62" t="n">
-        <v>0</v>
+        <v>0.0236976765386145</v>
       </c>
       <c r="E62" t="n">
         <v>0</v>
@@ -4838,13 +4865,13 @@
         <v>0</v>
       </c>
       <c r="L62" t="n">
-        <v>0.00643844708467661</v>
+        <v>0.00806459182920588</v>
       </c>
       <c r="M62" t="n">
         <v>0</v>
       </c>
       <c r="N62" t="n">
-        <v>0</v>
+        <v>0.00663259002640531</v>
       </c>
       <c r="O62" t="n">
         <v>0</v>
@@ -4876,7 +4903,7 @@
         <v>83</v>
       </c>
       <c r="B63" t="n">
-        <v>0.0107513627612623</v>
+        <v>0.0318315753938966</v>
       </c>
       <c r="C63" t="n">
         <v>0</v>
@@ -4903,25 +4930,25 @@
         <v>0</v>
       </c>
       <c r="K63" t="n">
-        <v>0</v>
+        <v>0.0194422766906005</v>
       </c>
       <c r="L63" t="n">
         <v>0</v>
       </c>
       <c r="M63" t="n">
-        <v>0</v>
+        <v>0.0459738131955484</v>
       </c>
       <c r="N63" t="n">
         <v>0</v>
       </c>
       <c r="O63" t="n">
-        <v>0</v>
+        <v>0.186128324385923</v>
       </c>
       <c r="P63" t="n">
         <v>0</v>
       </c>
       <c r="Q63" t="n">
-        <v>0</v>
+        <v>0.281930245346136</v>
       </c>
       <c r="R63" t="n">
         <v>0</v>
@@ -4944,7 +4971,7 @@
         <v>84</v>
       </c>
       <c r="B64" t="n">
-        <v>0.0086948066882848</v>
+        <v>0.0314748334346311</v>
       </c>
       <c r="C64" t="n">
         <v>0</v>
@@ -4974,7 +5001,7 @@
         <v>0</v>
       </c>
       <c r="L64" t="n">
-        <v>0</v>
+        <v>0.0112137190516242</v>
       </c>
       <c r="M64" t="n">
         <v>0</v>
@@ -5012,7 +5039,7 @@
         <v>85</v>
       </c>
       <c r="B65" t="n">
-        <v>0.00614363586357848</v>
+        <v>0.0270206552575152</v>
       </c>
       <c r="C65" t="n">
         <v>0</v>
@@ -5042,7 +5069,7 @@
         <v>0</v>
       </c>
       <c r="L65" t="n">
-        <v>0</v>
+        <v>0.03377237078914</v>
       </c>
       <c r="M65" t="n">
         <v>0</v>
@@ -5080,10 +5107,10 @@
         <v>86</v>
       </c>
       <c r="B66" t="n">
-        <v>0.00451661365394435</v>
+        <v>0.0129548294350441</v>
       </c>
       <c r="C66" t="n">
-        <v>0</v>
+        <v>0.00496335920150758</v>
       </c>
       <c r="D66" t="n">
         <v>0</v>
@@ -5092,13 +5119,13 @@
         <v>0</v>
       </c>
       <c r="F66" t="n">
-        <v>0</v>
+        <v>0.00839192965888644</v>
       </c>
       <c r="G66" t="n">
         <v>0</v>
       </c>
       <c r="H66" t="n">
-        <v>0</v>
+        <v>0.0425549789325351</v>
       </c>
       <c r="I66" t="n">
         <v>0</v>
@@ -5110,7 +5137,7 @@
         <v>0</v>
       </c>
       <c r="L66" t="n">
-        <v>0</v>
+        <v>0.0192379374549016</v>
       </c>
       <c r="M66" t="n">
         <v>0</v>
@@ -5119,16 +5146,16 @@
         <v>0</v>
       </c>
       <c r="O66" t="n">
-        <v>0</v>
+        <v>0.0637376519213384</v>
       </c>
       <c r="P66" t="n">
-        <v>0</v>
+        <v>0.00638486335041401</v>
       </c>
       <c r="Q66" t="n">
-        <v>0</v>
+        <v>0.00987546508033507</v>
       </c>
       <c r="R66" t="n">
-        <v>0</v>
+        <v>0.00338070521510787</v>
       </c>
       <c r="S66" t="n">
         <v>0</v>
@@ -5140,7 +5167,7 @@
         <v>0</v>
       </c>
       <c r="V66" t="n">
-        <v>0</v>
+        <v>0.00590401059439677</v>
       </c>
     </row>
     <row r="67">
@@ -5148,7 +5175,7 @@
         <v>87</v>
       </c>
       <c r="B67" t="n">
-        <v>0.00425629010040289</v>
+        <v>0.0122515381439205</v>
       </c>
       <c r="C67" t="n">
         <v>0</v>
@@ -5178,7 +5205,7 @@
         <v>0</v>
       </c>
       <c r="L67" t="n">
-        <v>0.00246376093515109</v>
+        <v>0.0352056274095996</v>
       </c>
       <c r="M67" t="n">
         <v>0</v>
@@ -5216,7 +5243,7 @@
         <v>88</v>
       </c>
       <c r="B68" t="n">
-        <v>0.00269434877915412</v>
+        <v>0.0113953574416831</v>
       </c>
       <c r="C68" t="n">
         <v>0</v>
@@ -5246,7 +5273,7 @@
         <v>0</v>
       </c>
       <c r="L68" t="n">
-        <v>0.0121962972259413</v>
+        <v>0.00902346069500632</v>
       </c>
       <c r="M68" t="n">
         <v>0</v>
@@ -5284,7 +5311,7 @@
         <v>89</v>
       </c>
       <c r="B69" t="n">
-        <v>0</v>
+        <v>0.00905105313793795</v>
       </c>
       <c r="C69" t="n">
         <v>0</v>
@@ -5296,40 +5323,40 @@
         <v>0</v>
       </c>
       <c r="F69" t="n">
-        <v>2.29749401393121</v>
+        <v>0</v>
       </c>
       <c r="G69" t="n">
-        <v>0.114302191807699</v>
+        <v>0</v>
       </c>
       <c r="H69" t="n">
-        <v>0.0733682345668145</v>
+        <v>0</v>
       </c>
       <c r="I69" t="n">
-        <v>1.06808357348703</v>
+        <v>0</v>
       </c>
       <c r="J69" t="n">
-        <v>14.4946988386399</v>
+        <v>0</v>
       </c>
       <c r="K69" t="n">
-        <v>0.0425717486005879</v>
+        <v>0</v>
       </c>
       <c r="L69" t="n">
-        <v>0</v>
+        <v>0.00477415761603802</v>
       </c>
       <c r="M69" t="n">
-        <v>4.49226395890172</v>
+        <v>0</v>
       </c>
       <c r="N69" t="n">
         <v>0</v>
       </c>
       <c r="O69" t="n">
-        <v>6.18566827601398</v>
+        <v>0</v>
       </c>
       <c r="P69" t="n">
         <v>0</v>
       </c>
       <c r="Q69" t="n">
-        <v>14.2040861629188</v>
+        <v>0</v>
       </c>
       <c r="R69" t="n">
         <v>0</v>
@@ -5352,16 +5379,16 @@
         <v>90</v>
       </c>
       <c r="B70" t="n">
-        <v>0</v>
+        <v>0.00841911023866751</v>
       </c>
       <c r="C70" t="n">
         <v>0</v>
       </c>
       <c r="D70" t="n">
-        <v>1.34233700193548</v>
+        <v>0</v>
       </c>
       <c r="E70" t="n">
-        <v>0.715334458277002</v>
+        <v>0</v>
       </c>
       <c r="F70" t="n">
         <v>0</v>
@@ -5391,7 +5418,7 @@
         <v>0</v>
       </c>
       <c r="O70" t="n">
-        <v>0.166987147049894</v>
+        <v>0</v>
       </c>
       <c r="P70" t="n">
         <v>0</v>
@@ -5400,19 +5427,19 @@
         <v>0</v>
       </c>
       <c r="R70" t="n">
-        <v>0.418864705030619</v>
+        <v>0</v>
       </c>
       <c r="S70" t="n">
-        <v>0.613260347595515</v>
+        <v>0</v>
       </c>
       <c r="T70" t="n">
-        <v>0.094263676739816</v>
+        <v>0</v>
       </c>
       <c r="U70" t="n">
         <v>0</v>
       </c>
       <c r="V70" t="n">
-        <v>1.1500680577277</v>
+        <v>0</v>
       </c>
     </row>
     <row r="71">
@@ -5420,7 +5447,7 @@
         <v>91</v>
       </c>
       <c r="B71" t="n">
-        <v>0</v>
+        <v>0.00680867510826864</v>
       </c>
       <c r="C71" t="n">
         <v>0</v>
@@ -5429,7 +5456,7 @@
         <v>0</v>
       </c>
       <c r="E71" t="n">
-        <v>1.49787479578247</v>
+        <v>0</v>
       </c>
       <c r="F71" t="n">
         <v>0</v>
@@ -5474,7 +5501,7 @@
         <v>0</v>
       </c>
       <c r="T71" t="n">
-        <v>0.128440750605615</v>
+        <v>0</v>
       </c>
       <c r="U71" t="n">
         <v>0</v>
@@ -5488,16 +5515,16 @@
         <v>92</v>
       </c>
       <c r="B72" t="n">
-        <v>0</v>
+        <v>0.0057588344852871</v>
       </c>
       <c r="C72" t="n">
         <v>0</v>
       </c>
       <c r="D72" t="n">
-        <v>0.602307815003416</v>
+        <v>0</v>
       </c>
       <c r="E72" t="n">
-        <v>0.919255658544931</v>
+        <v>0</v>
       </c>
       <c r="F72" t="n">
         <v>0</v>
@@ -5542,10 +5569,10 @@
         <v>0</v>
       </c>
       <c r="T72" t="n">
-        <v>0.00132554024989303</v>
+        <v>0</v>
       </c>
       <c r="U72" t="n">
-        <v>0.052307945408406</v>
+        <v>0</v>
       </c>
       <c r="V72" t="n">
         <v>0</v>
@@ -5556,7 +5583,7 @@
         <v>93</v>
       </c>
       <c r="B73" t="n">
-        <v>0</v>
+        <v>0.00481092013638143</v>
       </c>
       <c r="C73" t="n">
         <v>0</v>
@@ -5565,7 +5592,7 @@
         <v>0</v>
       </c>
       <c r="E73" t="n">
-        <v>0.00948262655336717</v>
+        <v>0</v>
       </c>
       <c r="F73" t="n">
         <v>0</v>
@@ -5610,13 +5637,13 @@
         <v>0</v>
       </c>
       <c r="T73" t="n">
-        <v>0.505440796111275</v>
+        <v>0</v>
       </c>
       <c r="U73" t="n">
         <v>0</v>
       </c>
       <c r="V73" t="n">
-        <v>0.047010529744146</v>
+        <v>0</v>
       </c>
     </row>
     <row r="74">
@@ -5624,7 +5651,7 @@
         <v>94</v>
       </c>
       <c r="B74" t="n">
-        <v>0</v>
+        <v>0.00353684171043296</v>
       </c>
       <c r="C74" t="n">
         <v>0</v>
@@ -5639,7 +5666,7 @@
         <v>0</v>
       </c>
       <c r="G74" t="n">
-        <v>0.414252546902544</v>
+        <v>0</v>
       </c>
       <c r="H74" t="n">
         <v>0</v>
@@ -5654,13 +5681,13 @@
         <v>0</v>
       </c>
       <c r="L74" t="n">
-        <v>0.0906146770458608</v>
+        <v>0</v>
       </c>
       <c r="M74" t="n">
-        <v>2.3560445913961</v>
+        <v>0</v>
       </c>
       <c r="N74" t="n">
-        <v>0.0971454552109843</v>
+        <v>0</v>
       </c>
       <c r="O74" t="n">
         <v>0</v>
@@ -5684,7 +5711,7 @@
         <v>0</v>
       </c>
       <c r="V74" t="n">
-        <v>0.0672616492120639</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75">
@@ -5692,7 +5719,7 @@
         <v>95</v>
       </c>
       <c r="B75" t="n">
-        <v>0</v>
+        <v>0.0033329891622812</v>
       </c>
       <c r="C75" t="n">
         <v>0</v>
@@ -5722,7 +5749,7 @@
         <v>0</v>
       </c>
       <c r="L75" t="n">
-        <v>0.166514848175156</v>
+        <v>0.00182689752326191</v>
       </c>
       <c r="M75" t="n">
         <v>0</v>
@@ -5760,7 +5787,7 @@
         <v>96</v>
       </c>
       <c r="B76" t="n">
-        <v>0</v>
+        <v>0.00210987387337067</v>
       </c>
       <c r="C76" t="n">
         <v>0</v>
@@ -5772,7 +5799,7 @@
         <v>0</v>
       </c>
       <c r="F76" t="n">
-        <v>0.475824444928167</v>
+        <v>0</v>
       </c>
       <c r="G76" t="n">
         <v>0</v>
@@ -5790,7 +5817,7 @@
         <v>0</v>
       </c>
       <c r="L76" t="n">
-        <v>0</v>
+        <v>0.00904364740797054</v>
       </c>
       <c r="M76" t="n">
         <v>0</v>
@@ -5799,7 +5826,7 @@
         <v>0</v>
       </c>
       <c r="O76" t="n">
-        <v>0.709918619811046</v>
+        <v>0</v>
       </c>
       <c r="P76" t="n">
         <v>0</v>
@@ -5814,7 +5841,7 @@
         <v>0</v>
       </c>
       <c r="T76" t="n">
-        <v>0.0205663719184435</v>
+        <v>0</v>
       </c>
       <c r="U76" t="n">
         <v>0</v>
@@ -5840,40 +5867,40 @@
         <v>0</v>
       </c>
       <c r="F77" t="n">
-        <v>0</v>
+        <v>0.0689628769413356</v>
       </c>
       <c r="G77" t="n">
-        <v>0</v>
+        <v>0.00769418794649928</v>
       </c>
       <c r="H77" t="n">
-        <v>0</v>
+        <v>0.021922564940098</v>
       </c>
       <c r="I77" t="n">
-        <v>0</v>
+        <v>0.0415132670941203</v>
       </c>
       <c r="J77" t="n">
-        <v>0.567717022331867</v>
+        <v>1.85402452149106</v>
       </c>
       <c r="K77" t="n">
-        <v>0</v>
+        <v>0.0238027873063936</v>
       </c>
       <c r="L77" t="n">
         <v>0</v>
       </c>
       <c r="M77" t="n">
-        <v>0</v>
+        <v>0.0748730726256759</v>
       </c>
       <c r="N77" t="n">
         <v>0</v>
       </c>
       <c r="O77" t="n">
-        <v>0</v>
+        <v>0.640386210109911</v>
       </c>
       <c r="P77" t="n">
         <v>0</v>
       </c>
       <c r="Q77" t="n">
-        <v>0</v>
+        <v>1.38392196750278</v>
       </c>
       <c r="R77" t="n">
         <v>0</v>
@@ -5902,10 +5929,10 @@
         <v>0</v>
       </c>
       <c r="D78" t="n">
-        <v>0</v>
+        <v>0.113718595032322</v>
       </c>
       <c r="E78" t="n">
-        <v>0</v>
+        <v>0.322758538570326</v>
       </c>
       <c r="F78" t="n">
         <v>0</v>
@@ -5926,7 +5953,7 @@
         <v>0</v>
       </c>
       <c r="L78" t="n">
-        <v>0.0693664404725412</v>
+        <v>0</v>
       </c>
       <c r="M78" t="n">
         <v>0</v>
@@ -5935,7 +5962,7 @@
         <v>0</v>
       </c>
       <c r="O78" t="n">
-        <v>0</v>
+        <v>0.0172877466855137</v>
       </c>
       <c r="P78" t="n">
         <v>0</v>
@@ -5944,19 +5971,19 @@
         <v>0</v>
       </c>
       <c r="R78" t="n">
-        <v>0</v>
+        <v>0.153061928718331</v>
       </c>
       <c r="S78" t="n">
-        <v>0</v>
+        <v>0.130721960829412</v>
       </c>
       <c r="T78" t="n">
-        <v>0</v>
+        <v>0.0690553739406562</v>
       </c>
       <c r="U78" t="n">
         <v>0</v>
       </c>
       <c r="V78" t="n">
-        <v>0</v>
+        <v>0.412009878310336</v>
       </c>
     </row>
     <row r="79">
@@ -5973,7 +6000,7 @@
         <v>0</v>
       </c>
       <c r="E79" t="n">
-        <v>0</v>
+        <v>0.675840335180479</v>
       </c>
       <c r="F79" t="n">
         <v>0</v>
@@ -5982,7 +6009,7 @@
         <v>0</v>
       </c>
       <c r="H79" t="n">
-        <v>0.0766483837399658</v>
+        <v>0</v>
       </c>
       <c r="I79" t="n">
         <v>0</v>
@@ -6018,7 +6045,7 @@
         <v>0</v>
       </c>
       <c r="T79" t="n">
-        <v>0</v>
+        <v>0.0940927021844343</v>
       </c>
       <c r="U79" t="n">
         <v>0</v>
@@ -6038,10 +6065,10 @@
         <v>0</v>
       </c>
       <c r="D80" t="n">
-        <v>0</v>
+        <v>0.0510256354405912</v>
       </c>
       <c r="E80" t="n">
-        <v>0</v>
+        <v>0.414767678938757</v>
       </c>
       <c r="F80" t="n">
         <v>0</v>
@@ -6068,7 +6095,7 @@
         <v>0</v>
       </c>
       <c r="N80" t="n">
-        <v>0.0460200706267206</v>
+        <v>0</v>
       </c>
       <c r="O80" t="n">
         <v>0</v>
@@ -6086,10 +6113,10 @@
         <v>0</v>
       </c>
       <c r="T80" t="n">
-        <v>0</v>
+        <v>0.000971059911893832</v>
       </c>
       <c r="U80" t="n">
-        <v>0</v>
+        <v>0.0290119933992942</v>
       </c>
       <c r="V80" t="n">
         <v>0</v>
@@ -6109,7 +6136,7 @@
         <v>0</v>
       </c>
       <c r="E81" t="n">
-        <v>0</v>
+        <v>0.00427855620927993</v>
       </c>
       <c r="F81" t="n">
         <v>0</v>
@@ -6130,7 +6157,7 @@
         <v>0</v>
       </c>
       <c r="L81" t="n">
-        <v>0.0168788041966152</v>
+        <v>0</v>
       </c>
       <c r="M81" t="n">
         <v>0</v>
@@ -6154,13 +6181,13 @@
         <v>0</v>
       </c>
       <c r="T81" t="n">
-        <v>0</v>
+        <v>0.370274154239352</v>
       </c>
       <c r="U81" t="n">
         <v>0</v>
       </c>
       <c r="V81" t="n">
-        <v>0</v>
+        <v>0.0168414403904572</v>
       </c>
     </row>
     <row r="82">
@@ -6180,7 +6207,7 @@
         <v>0</v>
       </c>
       <c r="F82" t="n">
-        <v>0.308486612973444</v>
+        <v>0.00680950983269739</v>
       </c>
       <c r="G82" t="n">
         <v>0</v>
@@ -6192,7 +6219,7 @@
         <v>0</v>
       </c>
       <c r="J82" t="n">
-        <v>0</v>
+        <v>0.055726916481717</v>
       </c>
       <c r="K82" t="n">
         <v>0</v>
@@ -6201,19 +6228,19 @@
         <v>0</v>
       </c>
       <c r="M82" t="n">
-        <v>0</v>
+        <v>0.00773925981959996</v>
       </c>
       <c r="N82" t="n">
         <v>0</v>
       </c>
       <c r="O82" t="n">
-        <v>0</v>
+        <v>0.0795359611324614</v>
       </c>
       <c r="P82" t="n">
         <v>0</v>
       </c>
       <c r="Q82" t="n">
-        <v>0</v>
+        <v>0.0776162586066004</v>
       </c>
       <c r="R82" t="n">
         <v>0</v>
@@ -6251,7 +6278,7 @@
         <v>0</v>
       </c>
       <c r="G83" t="n">
-        <v>0</v>
+        <v>0.0278851779023322</v>
       </c>
       <c r="H83" t="n">
         <v>0</v>
@@ -6266,13 +6293,13 @@
         <v>0</v>
       </c>
       <c r="L83" t="n">
-        <v>0.00857552148698998</v>
+        <v>0.0671914741014061</v>
       </c>
       <c r="M83" t="n">
-        <v>0</v>
+        <v>0.0392684622753243</v>
       </c>
       <c r="N83" t="n">
-        <v>0</v>
+        <v>0.0403557589238598</v>
       </c>
       <c r="O83" t="n">
         <v>0</v>
@@ -6296,6 +6323,618 @@
         <v>0</v>
       </c>
       <c r="V83" t="n">
+        <v>0.0240963686632329</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="s">
+        <v>104</v>
+      </c>
+      <c r="B84" t="n">
+        <v>0</v>
+      </c>
+      <c r="C84" t="n">
+        <v>0</v>
+      </c>
+      <c r="D84" t="n">
+        <v>0</v>
+      </c>
+      <c r="E84" t="n">
+        <v>0</v>
+      </c>
+      <c r="F84" t="n">
+        <v>0</v>
+      </c>
+      <c r="G84" t="n">
+        <v>0</v>
+      </c>
+      <c r="H84" t="n">
+        <v>0</v>
+      </c>
+      <c r="I84" t="n">
+        <v>0</v>
+      </c>
+      <c r="J84" t="n">
+        <v>0</v>
+      </c>
+      <c r="K84" t="n">
+        <v>0</v>
+      </c>
+      <c r="L84" t="n">
+        <v>0.123472029845651</v>
+      </c>
+      <c r="M84" t="n">
+        <v>0</v>
+      </c>
+      <c r="N84" t="n">
+        <v>0</v>
+      </c>
+      <c r="O84" t="n">
+        <v>0</v>
+      </c>
+      <c r="P84" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q84" t="n">
+        <v>0</v>
+      </c>
+      <c r="R84" t="n">
+        <v>0</v>
+      </c>
+      <c r="S84" t="n">
+        <v>0</v>
+      </c>
+      <c r="T84" t="n">
+        <v>0</v>
+      </c>
+      <c r="U84" t="n">
+        <v>0</v>
+      </c>
+      <c r="V84" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="s">
+        <v>105</v>
+      </c>
+      <c r="B85" t="n">
+        <v>0</v>
+      </c>
+      <c r="C85" t="n">
+        <v>0</v>
+      </c>
+      <c r="D85" t="n">
+        <v>0</v>
+      </c>
+      <c r="E85" t="n">
+        <v>0</v>
+      </c>
+      <c r="F85" t="n">
+        <v>0.0142826150763773</v>
+      </c>
+      <c r="G85" t="n">
+        <v>0</v>
+      </c>
+      <c r="H85" t="n">
+        <v>0</v>
+      </c>
+      <c r="I85" t="n">
+        <v>0</v>
+      </c>
+      <c r="J85" t="n">
+        <v>0</v>
+      </c>
+      <c r="K85" t="n">
+        <v>0</v>
+      </c>
+      <c r="L85" t="n">
+        <v>0</v>
+      </c>
+      <c r="M85" t="n">
+        <v>0</v>
+      </c>
+      <c r="N85" t="n">
+        <v>0</v>
+      </c>
+      <c r="O85" t="n">
+        <v>0.0734960353742427</v>
+      </c>
+      <c r="P85" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q85" t="n">
+        <v>0</v>
+      </c>
+      <c r="R85" t="n">
+        <v>0</v>
+      </c>
+      <c r="S85" t="n">
+        <v>0</v>
+      </c>
+      <c r="T85" t="n">
+        <v>0.0150664450247445</v>
+      </c>
+      <c r="U85" t="n">
+        <v>0</v>
+      </c>
+      <c r="V85" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="s">
+        <v>106</v>
+      </c>
+      <c r="B86" t="n">
+        <v>0</v>
+      </c>
+      <c r="C86" t="n">
+        <v>0</v>
+      </c>
+      <c r="D86" t="n">
+        <v>0</v>
+      </c>
+      <c r="E86" t="n">
+        <v>0</v>
+      </c>
+      <c r="F86" t="n">
+        <v>0</v>
+      </c>
+      <c r="G86" t="n">
+        <v>0</v>
+      </c>
+      <c r="H86" t="n">
+        <v>0</v>
+      </c>
+      <c r="I86" t="n">
+        <v>0</v>
+      </c>
+      <c r="J86" t="n">
+        <v>0.0726169817247434</v>
+      </c>
+      <c r="K86" t="n">
+        <v>0</v>
+      </c>
+      <c r="L86" t="n">
+        <v>0</v>
+      </c>
+      <c r="M86" t="n">
+        <v>0</v>
+      </c>
+      <c r="N86" t="n">
+        <v>0</v>
+      </c>
+      <c r="O86" t="n">
+        <v>0</v>
+      </c>
+      <c r="P86" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q86" t="n">
+        <v>0</v>
+      </c>
+      <c r="R86" t="n">
+        <v>0</v>
+      </c>
+      <c r="S86" t="n">
+        <v>0</v>
+      </c>
+      <c r="T86" t="n">
+        <v>0</v>
+      </c>
+      <c r="U86" t="n">
+        <v>0</v>
+      </c>
+      <c r="V86" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="s">
+        <v>107</v>
+      </c>
+      <c r="B87" t="n">
+        <v>0</v>
+      </c>
+      <c r="C87" t="n">
+        <v>0</v>
+      </c>
+      <c r="D87" t="n">
+        <v>0</v>
+      </c>
+      <c r="E87" t="n">
+        <v>0</v>
+      </c>
+      <c r="F87" t="n">
+        <v>0</v>
+      </c>
+      <c r="G87" t="n">
+        <v>0</v>
+      </c>
+      <c r="H87" t="n">
+        <v>0</v>
+      </c>
+      <c r="I87" t="n">
+        <v>0</v>
+      </c>
+      <c r="J87" t="n">
+        <v>0</v>
+      </c>
+      <c r="K87" t="n">
+        <v>0</v>
+      </c>
+      <c r="L87" t="n">
+        <v>0.0514357446328325</v>
+      </c>
+      <c r="M87" t="n">
+        <v>0</v>
+      </c>
+      <c r="N87" t="n">
+        <v>0</v>
+      </c>
+      <c r="O87" t="n">
+        <v>0</v>
+      </c>
+      <c r="P87" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q87" t="n">
+        <v>0</v>
+      </c>
+      <c r="R87" t="n">
+        <v>0</v>
+      </c>
+      <c r="S87" t="n">
+        <v>0</v>
+      </c>
+      <c r="T87" t="n">
+        <v>0</v>
+      </c>
+      <c r="U87" t="n">
+        <v>0</v>
+      </c>
+      <c r="V87" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="s">
+        <v>108</v>
+      </c>
+      <c r="B88" t="n">
+        <v>0</v>
+      </c>
+      <c r="C88" t="n">
+        <v>0</v>
+      </c>
+      <c r="D88" t="n">
+        <v>0</v>
+      </c>
+      <c r="E88" t="n">
+        <v>0</v>
+      </c>
+      <c r="F88" t="n">
+        <v>0</v>
+      </c>
+      <c r="G88" t="n">
+        <v>0</v>
+      </c>
+      <c r="H88" t="n">
+        <v>0.0229026796135148</v>
+      </c>
+      <c r="I88" t="n">
+        <v>0</v>
+      </c>
+      <c r="J88" t="n">
+        <v>0</v>
+      </c>
+      <c r="K88" t="n">
+        <v>0</v>
+      </c>
+      <c r="L88" t="n">
+        <v>0</v>
+      </c>
+      <c r="M88" t="n">
+        <v>0</v>
+      </c>
+      <c r="N88" t="n">
+        <v>0</v>
+      </c>
+      <c r="O88" t="n">
+        <v>0</v>
+      </c>
+      <c r="P88" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q88" t="n">
+        <v>0</v>
+      </c>
+      <c r="R88" t="n">
+        <v>0</v>
+      </c>
+      <c r="S88" t="n">
+        <v>0</v>
+      </c>
+      <c r="T88" t="n">
+        <v>0</v>
+      </c>
+      <c r="U88" t="n">
+        <v>0</v>
+      </c>
+      <c r="V88" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="s">
+        <v>109</v>
+      </c>
+      <c r="B89" t="n">
+        <v>0</v>
+      </c>
+      <c r="C89" t="n">
+        <v>0</v>
+      </c>
+      <c r="D89" t="n">
+        <v>0</v>
+      </c>
+      <c r="E89" t="n">
+        <v>0</v>
+      </c>
+      <c r="F89" t="n">
+        <v>0</v>
+      </c>
+      <c r="G89" t="n">
+        <v>0</v>
+      </c>
+      <c r="H89" t="n">
+        <v>0</v>
+      </c>
+      <c r="I89" t="n">
+        <v>0</v>
+      </c>
+      <c r="J89" t="n">
+        <v>0</v>
+      </c>
+      <c r="K89" t="n">
+        <v>0</v>
+      </c>
+      <c r="L89" t="n">
+        <v>0</v>
+      </c>
+      <c r="M89" t="n">
+        <v>0</v>
+      </c>
+      <c r="N89" t="n">
+        <v>0.0191174653702271</v>
+      </c>
+      <c r="O89" t="n">
+        <v>0</v>
+      </c>
+      <c r="P89" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q89" t="n">
+        <v>0</v>
+      </c>
+      <c r="R89" t="n">
+        <v>0</v>
+      </c>
+      <c r="S89" t="n">
+        <v>0</v>
+      </c>
+      <c r="T89" t="n">
+        <v>0</v>
+      </c>
+      <c r="U89" t="n">
+        <v>0</v>
+      </c>
+      <c r="V89" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="s">
+        <v>110</v>
+      </c>
+      <c r="B90" t="n">
+        <v>0</v>
+      </c>
+      <c r="C90" t="n">
+        <v>0</v>
+      </c>
+      <c r="D90" t="n">
+        <v>0</v>
+      </c>
+      <c r="E90" t="n">
+        <v>0</v>
+      </c>
+      <c r="F90" t="n">
+        <v>0</v>
+      </c>
+      <c r="G90" t="n">
+        <v>0</v>
+      </c>
+      <c r="H90" t="n">
+        <v>0</v>
+      </c>
+      <c r="I90" t="n">
+        <v>0</v>
+      </c>
+      <c r="J90" t="n">
+        <v>0</v>
+      </c>
+      <c r="K90" t="n">
+        <v>0</v>
+      </c>
+      <c r="L90" t="n">
+        <v>0.0125157620378164</v>
+      </c>
+      <c r="M90" t="n">
+        <v>0</v>
+      </c>
+      <c r="N90" t="n">
+        <v>0</v>
+      </c>
+      <c r="O90" t="n">
+        <v>0</v>
+      </c>
+      <c r="P90" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q90" t="n">
+        <v>0</v>
+      </c>
+      <c r="R90" t="n">
+        <v>0</v>
+      </c>
+      <c r="S90" t="n">
+        <v>0</v>
+      </c>
+      <c r="T90" t="n">
+        <v>0</v>
+      </c>
+      <c r="U90" t="n">
+        <v>0</v>
+      </c>
+      <c r="V90" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="s">
+        <v>111</v>
+      </c>
+      <c r="B91" t="n">
+        <v>0</v>
+      </c>
+      <c r="C91" t="n">
+        <v>0</v>
+      </c>
+      <c r="D91" t="n">
+        <v>0</v>
+      </c>
+      <c r="E91" t="n">
+        <v>0</v>
+      </c>
+      <c r="F91" t="n">
+        <v>0.00925970827324817</v>
+      </c>
+      <c r="G91" t="n">
+        <v>0</v>
+      </c>
+      <c r="H91" t="n">
+        <v>0</v>
+      </c>
+      <c r="I91" t="n">
+        <v>0</v>
+      </c>
+      <c r="J91" t="n">
+        <v>0</v>
+      </c>
+      <c r="K91" t="n">
+        <v>0</v>
+      </c>
+      <c r="L91" t="n">
+        <v>0</v>
+      </c>
+      <c r="M91" t="n">
+        <v>0</v>
+      </c>
+      <c r="N91" t="n">
+        <v>0</v>
+      </c>
+      <c r="O91" t="n">
+        <v>0</v>
+      </c>
+      <c r="P91" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q91" t="n">
+        <v>0</v>
+      </c>
+      <c r="R91" t="n">
+        <v>0</v>
+      </c>
+      <c r="S91" t="n">
+        <v>0</v>
+      </c>
+      <c r="T91" t="n">
+        <v>0</v>
+      </c>
+      <c r="U91" t="n">
+        <v>0</v>
+      </c>
+      <c r="V91" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="s">
+        <v>112</v>
+      </c>
+      <c r="B92" t="n">
+        <v>0</v>
+      </c>
+      <c r="C92" t="n">
+        <v>0</v>
+      </c>
+      <c r="D92" t="n">
+        <v>0</v>
+      </c>
+      <c r="E92" t="n">
+        <v>0</v>
+      </c>
+      <c r="F92" t="n">
+        <v>0</v>
+      </c>
+      <c r="G92" t="n">
+        <v>0</v>
+      </c>
+      <c r="H92" t="n">
+        <v>0</v>
+      </c>
+      <c r="I92" t="n">
+        <v>0</v>
+      </c>
+      <c r="J92" t="n">
+        <v>0</v>
+      </c>
+      <c r="K92" t="n">
+        <v>0</v>
+      </c>
+      <c r="L92" t="n">
+        <v>0.00635881458372929</v>
+      </c>
+      <c r="M92" t="n">
+        <v>0</v>
+      </c>
+      <c r="N92" t="n">
+        <v>0</v>
+      </c>
+      <c r="O92" t="n">
+        <v>0</v>
+      </c>
+      <c r="P92" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q92" t="n">
+        <v>0</v>
+      </c>
+      <c r="R92" t="n">
+        <v>0</v>
+      </c>
+      <c r="S92" t="n">
+        <v>0</v>
+      </c>
+      <c r="T92" t="n">
+        <v>0</v>
+      </c>
+      <c r="U92" t="n">
+        <v>0</v>
+      </c>
+      <c r="V92" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Filtering out Partitiviridae family from test
</commit_message>
<xml_diff>
--- a/test/pivot_filtering/LakeVarese_MetaPhlAn_filtered_family_scaling.xlsx
+++ b/test/pivot_filtering/LakeVarese_MetaPhlAn_filtered_family_scaling.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="116">
   <si>
     <t xml:space="preserve">family</t>
   </si>
@@ -315,9 +315,6 @@
   </si>
   <si>
     <t xml:space="preserve">Helicobacteraceae</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Partitiviridae</t>
   </si>
   <si>
     <t xml:space="preserve">Rhodospirillales_noname</t>
@@ -791,7 +788,7 @@
         <v>48.0244018977011</v>
       </c>
       <c r="G2" t="n">
-        <v>75.8675805194696</v>
+        <v>76.0453023843103</v>
       </c>
       <c r="H2" t="n">
         <v>37.9792909131016</v>
@@ -868,7 +865,7 @@
         <v>4.9580090989956</v>
       </c>
       <c r="G3" t="n">
-        <v>8.49930305483025</v>
+        <v>8.51921290273114</v>
       </c>
       <c r="H3" t="n">
         <v>16.8949174652702</v>
@@ -945,7 +942,7 @@
         <v>2.92312171130139</v>
       </c>
       <c r="G4" t="n">
-        <v>1.84841272174407</v>
+        <v>1.85274267867237</v>
       </c>
       <c r="H4" t="n">
         <v>36.6696595020355</v>
@@ -1022,7 +1019,7 @@
         <v>0.077992832409256</v>
       </c>
       <c r="G5" t="n">
-        <v>1.0213860394706</v>
+        <v>1.02377866396731</v>
       </c>
       <c r="H5" t="n">
         <v>0.581056902720512</v>
@@ -1099,7 +1096,7 @@
         <v>0.112604737592818</v>
       </c>
       <c r="G6" t="n">
-        <v>0.631945102102493</v>
+        <v>0.633425450642061</v>
       </c>
       <c r="H6" t="n">
         <v>0.861566441695482</v>
@@ -1176,7 +1173,7 @@
         <v>1.66321808981638</v>
       </c>
       <c r="G7" t="n">
-        <v>2.50346895900917</v>
+        <v>2.50933340293791</v>
       </c>
       <c r="H7" t="n">
         <v>2.99812076615919</v>
@@ -1407,7 +1404,7 @@
         <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>0.0664343414379297</v>
+        <v>0.0665899656843993</v>
       </c>
       <c r="H10" t="n">
         <v>0.1219776322654</v>
@@ -1484,7 +1481,7 @@
         <v>0.0715447252919686</v>
       </c>
       <c r="G11" t="n">
-        <v>0.0899828792466584</v>
+        <v>0.0901936665815642</v>
       </c>
       <c r="H11" t="n">
         <v>0.396044655437949</v>
@@ -1561,7 +1558,7 @@
         <v>0.185986012955751</v>
       </c>
       <c r="G12" t="n">
-        <v>0.207695051826619</v>
+        <v>0.208181583118062</v>
       </c>
       <c r="H12" t="n">
         <v>0.0977981901932705</v>
@@ -1715,7 +1712,7 @@
         <v>24.4707683287949</v>
       </c>
       <c r="G14" t="n">
-        <v>0.786266858947513</v>
+        <v>0.788108710387586</v>
       </c>
       <c r="H14" t="n">
         <v>0.251178085042209</v>
@@ -2254,7 +2251,7 @@
         <v>0.196803494692421</v>
       </c>
       <c r="G21" t="n">
-        <v>0.262563653528685</v>
+        <v>0.263178716007612</v>
       </c>
       <c r="H21" t="n">
         <v>0.470143591072314</v>
@@ -3101,7 +3098,7 @@
         <v>15.3091988453953</v>
       </c>
       <c r="G32" t="n">
-        <v>6.76238731922937</v>
+        <v>6.77822839491571</v>
       </c>
       <c r="H32" t="n">
         <v>0.145516824319897</v>
@@ -6181,7 +6178,7 @@
         <v>0.675840335180479</v>
       </c>
       <c r="G72" t="n">
-        <v>0.125626108828423</v>
+        <v>0.125920391395243</v>
       </c>
       <c r="H72" t="n">
         <v>0</v>
@@ -6258,7 +6255,7 @@
         <v>0.322758538570326</v>
       </c>
       <c r="G73" t="n">
-        <v>0.741489034569966</v>
+        <v>0.743225992742091</v>
       </c>
       <c r="H73" t="n">
         <v>0</v>
@@ -6335,7 +6332,7 @@
         <v>0.414767678938757</v>
       </c>
       <c r="G74" t="n">
-        <v>0.351753104719585</v>
+        <v>0.35257709590668</v>
       </c>
       <c r="H74" t="n">
         <v>0</v>
@@ -6643,7 +6640,7 @@
         <v>0</v>
       </c>
       <c r="G78" t="n">
-        <v>0.233705251039111</v>
+        <v>0</v>
       </c>
       <c r="H78" t="n">
         <v>0</v>
@@ -6661,16 +6658,16 @@
         <v>0</v>
       </c>
       <c r="M78" t="n">
-        <v>0</v>
+        <v>0.0795359611324614</v>
       </c>
       <c r="N78" t="n">
         <v>0</v>
       </c>
       <c r="O78" t="n">
-        <v>0</v>
+        <v>0.0776162586066004</v>
       </c>
       <c r="P78" t="n">
-        <v>0</v>
+        <v>0.00773925981959996</v>
       </c>
       <c r="Q78" t="n">
         <v>0</v>
@@ -6688,7 +6685,7 @@
         <v>0</v>
       </c>
       <c r="V78" t="n">
-        <v>0</v>
+        <v>0.055726916481717</v>
       </c>
       <c r="W78" t="n">
         <v>0</v>
@@ -6697,7 +6694,7 @@
         <v>0</v>
       </c>
       <c r="Y78" t="n">
-        <v>0</v>
+        <v>0.00680950983269739</v>
       </c>
     </row>
     <row r="79">
@@ -6723,7 +6720,7 @@
         <v>0</v>
       </c>
       <c r="H79" t="n">
-        <v>0</v>
+        <v>0.0120947229893273</v>
       </c>
       <c r="I79" t="n">
         <v>0</v>
@@ -6738,16 +6735,16 @@
         <v>0</v>
       </c>
       <c r="M79" t="n">
-        <v>0.0795359611324614</v>
+        <v>0</v>
       </c>
       <c r="N79" t="n">
         <v>0</v>
       </c>
       <c r="O79" t="n">
-        <v>0.0776162586066004</v>
+        <v>0</v>
       </c>
       <c r="P79" t="n">
-        <v>0.00773925981959996</v>
+        <v>0</v>
       </c>
       <c r="Q79" t="n">
         <v>0</v>
@@ -6759,22 +6756,22 @@
         <v>0</v>
       </c>
       <c r="T79" t="n">
-        <v>0</v>
+        <v>0.0410355179429484</v>
       </c>
       <c r="U79" t="n">
-        <v>0</v>
+        <v>0.0681379721427407</v>
       </c>
       <c r="V79" t="n">
-        <v>0.055726916481717</v>
+        <v>0.0216584190281003</v>
       </c>
       <c r="W79" t="n">
-        <v>0</v>
+        <v>0.0684580164337244</v>
       </c>
       <c r="X79" t="n">
         <v>0</v>
       </c>
       <c r="Y79" t="n">
-        <v>0.00680950983269739</v>
+        <v>0</v>
       </c>
     </row>
     <row r="80">
@@ -6800,7 +6797,7 @@
         <v>0</v>
       </c>
       <c r="H80" t="n">
-        <v>0.0120947229893273</v>
+        <v>0.00764298458548063</v>
       </c>
       <c r="I80" t="n">
         <v>0</v>
@@ -6836,16 +6833,16 @@
         <v>0</v>
       </c>
       <c r="T80" t="n">
-        <v>0.0410355179429484</v>
+        <v>0.0965037962950411</v>
       </c>
       <c r="U80" t="n">
-        <v>0.0681379721427407</v>
+        <v>0</v>
       </c>
       <c r="V80" t="n">
-        <v>0.0216584190281003</v>
+        <v>0</v>
       </c>
       <c r="W80" t="n">
-        <v>0.0684580164337244</v>
+        <v>0</v>
       </c>
       <c r="X80" t="n">
         <v>0</v>
@@ -6877,7 +6874,7 @@
         <v>0</v>
       </c>
       <c r="H81" t="n">
-        <v>0.00764298458548063</v>
+        <v>0</v>
       </c>
       <c r="I81" t="n">
         <v>0</v>
@@ -6892,7 +6889,7 @@
         <v>0</v>
       </c>
       <c r="M81" t="n">
-        <v>0</v>
+        <v>0.0734960353742427</v>
       </c>
       <c r="N81" t="n">
         <v>0</v>
@@ -6904,7 +6901,7 @@
         <v>0</v>
       </c>
       <c r="Q81" t="n">
-        <v>0</v>
+        <v>0.0150664450247445</v>
       </c>
       <c r="R81" t="n">
         <v>0</v>
@@ -6913,7 +6910,7 @@
         <v>0</v>
       </c>
       <c r="T81" t="n">
-        <v>0.0965037962950411</v>
+        <v>0</v>
       </c>
       <c r="U81" t="n">
         <v>0</v>
@@ -6928,7 +6925,7 @@
         <v>0</v>
       </c>
       <c r="Y81" t="n">
-        <v>0</v>
+        <v>0.0142826150763773</v>
       </c>
     </row>
     <row r="82">
@@ -6969,7 +6966,7 @@
         <v>0</v>
       </c>
       <c r="M82" t="n">
-        <v>0.0734960353742427</v>
+        <v>0</v>
       </c>
       <c r="N82" t="n">
         <v>0</v>
@@ -6981,7 +6978,7 @@
         <v>0</v>
       </c>
       <c r="Q82" t="n">
-        <v>0.0150664450247445</v>
+        <v>0</v>
       </c>
       <c r="R82" t="n">
         <v>0</v>
@@ -6996,7 +6993,7 @@
         <v>0</v>
       </c>
       <c r="V82" t="n">
-        <v>0</v>
+        <v>0.0726169817247434</v>
       </c>
       <c r="W82" t="n">
         <v>0</v>
@@ -7005,7 +7002,7 @@
         <v>0</v>
       </c>
       <c r="Y82" t="n">
-        <v>0.0142826150763773</v>
+        <v>0</v>
       </c>
     </row>
     <row r="83">
@@ -7067,13 +7064,13 @@
         <v>0</v>
       </c>
       <c r="T83" t="n">
-        <v>0</v>
+        <v>0.0648760734492962</v>
       </c>
       <c r="U83" t="n">
         <v>0</v>
       </c>
       <c r="V83" t="n">
-        <v>0.0726169817247434</v>
+        <v>0</v>
       </c>
       <c r="W83" t="n">
         <v>0</v>
@@ -7144,7 +7141,7 @@
         <v>0</v>
       </c>
       <c r="T84" t="n">
-        <v>0.0648760734492962</v>
+        <v>0.050045800571256</v>
       </c>
       <c r="U84" t="n">
         <v>0</v>
@@ -7221,10 +7218,10 @@
         <v>0</v>
       </c>
       <c r="T85" t="n">
-        <v>0.050045800571256</v>
+        <v>0</v>
       </c>
       <c r="U85" t="n">
-        <v>0</v>
+        <v>0.0229026796135148</v>
       </c>
       <c r="V85" t="n">
         <v>0</v>
@@ -7262,7 +7259,7 @@
         <v>0</v>
       </c>
       <c r="H86" t="n">
-        <v>0</v>
+        <v>0.0191174653702271</v>
       </c>
       <c r="I86" t="n">
         <v>0</v>
@@ -7301,7 +7298,7 @@
         <v>0</v>
       </c>
       <c r="U86" t="n">
-        <v>0.0229026796135148</v>
+        <v>0</v>
       </c>
       <c r="V86" t="n">
         <v>0</v>
@@ -7339,7 +7336,7 @@
         <v>0</v>
       </c>
       <c r="H87" t="n">
-        <v>0.0191174653702271</v>
+        <v>0</v>
       </c>
       <c r="I87" t="n">
         <v>0</v>
@@ -7390,7 +7387,7 @@
         <v>0</v>
       </c>
       <c r="Y87" t="n">
-        <v>0</v>
+        <v>0.00925970827324817</v>
       </c>
     </row>
     <row r="88">
@@ -7452,7 +7449,7 @@
         <v>0</v>
       </c>
       <c r="T88" t="n">
-        <v>0</v>
+        <v>0.00841911023866751</v>
       </c>
       <c r="U88" t="n">
         <v>0</v>
@@ -7467,7 +7464,7 @@
         <v>0</v>
       </c>
       <c r="Y88" t="n">
-        <v>0.00925970827324817</v>
+        <v>0</v>
       </c>
     </row>
     <row r="89">
@@ -7529,7 +7526,7 @@
         <v>0</v>
       </c>
       <c r="T89" t="n">
-        <v>0.00841911023866751</v>
+        <v>0.00680867510826864</v>
       </c>
       <c r="U89" t="n">
         <v>0</v>
@@ -7606,7 +7603,7 @@
         <v>0</v>
       </c>
       <c r="T90" t="n">
-        <v>0.00680867510826864</v>
+        <v>0.0057588344852871</v>
       </c>
       <c r="U90" t="n">
         <v>0</v>
@@ -7683,7 +7680,7 @@
         <v>0</v>
       </c>
       <c r="T91" t="n">
-        <v>0.0057588344852871</v>
+        <v>0.00481092013638143</v>
       </c>
       <c r="U91" t="n">
         <v>0</v>
@@ -7760,7 +7757,7 @@
         <v>0</v>
       </c>
       <c r="T92" t="n">
-        <v>0.00481092013638143</v>
+        <v>0.00353684171043296</v>
       </c>
       <c r="U92" t="n">
         <v>0</v>
@@ -7775,83 +7772,6 @@
         <v>0</v>
       </c>
       <c r="Y92" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" t="s">
-        <v>116</v>
-      </c>
-      <c r="B93" t="n">
-        <v>0</v>
-      </c>
-      <c r="C93" t="n">
-        <v>0</v>
-      </c>
-      <c r="D93" t="n">
-        <v>0</v>
-      </c>
-      <c r="E93" t="n">
-        <v>0</v>
-      </c>
-      <c r="F93" t="n">
-        <v>0</v>
-      </c>
-      <c r="G93" t="n">
-        <v>0</v>
-      </c>
-      <c r="H93" t="n">
-        <v>0</v>
-      </c>
-      <c r="I93" t="n">
-        <v>0</v>
-      </c>
-      <c r="J93" t="n">
-        <v>0</v>
-      </c>
-      <c r="K93" t="n">
-        <v>0</v>
-      </c>
-      <c r="L93" t="n">
-        <v>0</v>
-      </c>
-      <c r="M93" t="n">
-        <v>0</v>
-      </c>
-      <c r="N93" t="n">
-        <v>0</v>
-      </c>
-      <c r="O93" t="n">
-        <v>0</v>
-      </c>
-      <c r="P93" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q93" t="n">
-        <v>0</v>
-      </c>
-      <c r="R93" t="n">
-        <v>0</v>
-      </c>
-      <c r="S93" t="n">
-        <v>0</v>
-      </c>
-      <c r="T93" t="n">
-        <v>0.00353684171043296</v>
-      </c>
-      <c r="U93" t="n">
-        <v>0</v>
-      </c>
-      <c r="V93" t="n">
-        <v>0</v>
-      </c>
-      <c r="W93" t="n">
-        <v>0</v>
-      </c>
-      <c r="X93" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y93" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>